<commit_message>
Preparatory work for enabling font classes
</commit_message>
<xml_diff>
--- a/BigAsciiChars.xlsx
+++ b/BigAsciiChars.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DavidJohnson\Dropbox (Crisp)\WindowsPowerShell\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidjohnson\Documents\PowerShell\Modules\BigAsciiChars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BB5648-0EED-4847-BE90-1A634D29AF36}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D328DB-C1BF-4C88-84ED-6390CECB8F4C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="7308" xr2:uid="{6D1A8F03-DA32-4E55-9CE4-87A60CFBC80E}"/>
+    <workbookView xWindow="24225" yWindow="5355" windowWidth="12075" windowHeight="15375" xr2:uid="{6D1A8F03-DA32-4E55-9CE4-87A60CFBC80E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Code</t>
   </si>
@@ -39,13 +45,16 @@
     <t>Width</t>
   </si>
   <si>
-    <t>K</t>
+    <t>Put a 1 in each box</t>
   </si>
   <si>
-    <t>~</t>
+    <t>Draw your character here ==&gt;</t>
   </si>
   <si>
-    <t>2=3</t>
+    <t>&lt;== This is your value to use</t>
+  </si>
+  <si>
+    <t>FontValue</t>
   </si>
 </sst>
 </file>
@@ -409,18 +418,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E59BF4F4-332D-4568-800C-714E5C383342}">
-  <dimension ref="A1:P98"/>
+  <dimension ref="A1:Q98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="14" width="1.77734375" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+    <col min="10" max="14" width="1.7109375" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,11 +446,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>32</v>
       </c>
@@ -471,7 +484,7 @@
         <v>31457280</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:17" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>33</v>
       </c>
@@ -485,33 +498,33 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="H3" s="1"/>
+      <c r="E3">
+        <f>_xlfn.BITLSHIFT(D3,25)+C3</f>
+        <v>34636801</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="I3" s="1">
         <v>3</v>
       </c>
-      <c r="J3" s="2">
-        <v>1</v>
-      </c>
+      <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="2">
-        <v>1</v>
-      </c>
-      <c r="M3" s="2">
-        <v>1</v>
-      </c>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
       <c r="N3" s="2">
         <v>1</v>
       </c>
       <c r="O3">
         <f t="shared" ref="O3:O6" si="1">N3+2*M3+4*L3+8*K3+16*J3</f>
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="P3">
         <f t="shared" ref="P3:P6" si="2">_xlfn.BITLSHIFT(O3,5*I3)</f>
-        <v>753664</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="16.8" x14ac:dyDescent="0.5">
+        <v>32768</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>34</v>
       </c>
@@ -525,14 +538,20 @@
       <c r="D4">
         <v>3</v>
       </c>
-      <c r="H4" s="1"/>
+      <c r="E4">
+        <f>_xlfn.BITLSHIFT(D4,25)+C4</f>
+        <v>106070016</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="I4" s="1">
         <v>2</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="2"/>
+      <c r="K4" s="2">
         <v>1</v>
       </c>
-      <c r="K4" s="2"/>
       <c r="L4" s="2">
         <v>1</v>
       </c>
@@ -544,14 +563,14 @@
       </c>
       <c r="O4">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="P4">
         <f t="shared" si="2"/>
-        <v>23552</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="16.8" x14ac:dyDescent="0.5">
+        <v>15360</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>35</v>
       </c>
@@ -564,6 +583,10 @@
       </c>
       <c r="D5">
         <v>5</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E68" si="3">_xlfn.BITLSHIFT(D5,25)+C5</f>
+        <v>179284970</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1">
@@ -575,17 +598,19 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
+      <c r="N5" s="2">
+        <v>1</v>
+      </c>
       <c r="O5">
         <f>N5+2*M5+4*L5+8*K5+16*J5</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P5">
         <f t="shared" si="2"/>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="16.8" x14ac:dyDescent="0.5">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>36</v>
       </c>
@@ -598,6 +623,10 @@
       </c>
       <c r="D6">
         <v>5</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="3"/>
+        <v>184170686</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1">
@@ -625,7 +654,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>37</v>
       </c>
@@ -639,12 +668,19 @@
       <c r="D7">
         <v>5</v>
       </c>
+      <c r="E7">
+        <f t="shared" si="3"/>
+        <v>194842995</v>
+      </c>
       <c r="P7">
         <f>SUM(P2:P6)</f>
-        <v>32235023</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="16.8" x14ac:dyDescent="0.5">
+        <v>31505967</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>38</v>
       </c>
@@ -658,11 +694,13 @@
       <c r="D8">
         <v>5</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>180957773</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>39</v>
       </c>
@@ -676,11 +714,12 @@
       <c r="D9">
         <v>2</v>
       </c>
-      <c r="P9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>68222976</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>40</v>
       </c>
@@ -694,8 +733,12 @@
       <c r="D10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <f t="shared" si="3"/>
+        <v>68225089</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>41</v>
       </c>
@@ -709,8 +752,12 @@
       <c r="D11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <f t="shared" si="3"/>
+        <v>69239842</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>42</v>
       </c>
@@ -724,8 +771,12 @@
       <c r="D12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <f t="shared" si="3"/>
+        <v>185750673</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>43</v>
       </c>
@@ -739,8 +790,12 @@
       <c r="D13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <f t="shared" si="3"/>
+        <v>172129412</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>44</v>
       </c>
@@ -754,8 +809,12 @@
       <c r="D14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <f t="shared" si="3"/>
+        <v>67108898</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>45</v>
       </c>
@@ -769,8 +828,12 @@
       <c r="D15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <f t="shared" si="3"/>
+        <v>100670464</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>46</v>
       </c>
@@ -784,8 +847,12 @@
       <c r="D16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <f t="shared" si="3"/>
+        <v>67108963</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>47</v>
       </c>
@@ -799,8 +866,12 @@
       <c r="D17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <f t="shared" si="3"/>
+        <v>168890640</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>48</v>
       </c>
@@ -814,8 +885,12 @@
       <c r="D18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <f t="shared" si="3"/>
+        <v>140813606</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>49</v>
       </c>
@@ -829,8 +904,12 @@
       <c r="D19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <f t="shared" si="3"/>
+        <v>107022407</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>50</v>
       </c>
@@ -844,8 +923,12 @@
       <c r="D20">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <f t="shared" si="3"/>
+        <v>140806287</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>51</v>
       </c>
@@ -859,8 +942,12 @@
       <c r="D21">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <f t="shared" si="3"/>
+        <v>183015982</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>52</v>
       </c>
@@ -874,8 +961,12 @@
       <c r="D22">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <f t="shared" si="3"/>
+        <v>142949442</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>53</v>
       </c>
@@ -889,8 +980,12 @@
       <c r="D23">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <f t="shared" si="3"/>
+        <v>150222894</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>54</v>
       </c>
@@ -904,8 +999,12 @@
       <c r="D24">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <f t="shared" si="3"/>
+        <v>141834534</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>55</v>
       </c>
@@ -919,8 +1018,12 @@
       <c r="D25">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25">
+        <f t="shared" si="3"/>
+        <v>150016264</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>56</v>
       </c>
@@ -934,8 +1037,12 @@
       <c r="D26">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <f t="shared" si="3"/>
+        <v>140810534</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>57</v>
       </c>
@@ -949,8 +1056,12 @@
       <c r="D27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27">
+        <f t="shared" si="3"/>
+        <v>140811302</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>58</v>
       </c>
@@ -964,8 +1075,12 @@
       <c r="D28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28">
+        <f t="shared" si="3"/>
+        <v>33587201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>59</v>
       </c>
@@ -979,8 +1094,12 @@
       <c r="D29">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29">
+        <f t="shared" si="3"/>
+        <v>67141666</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>60</v>
       </c>
@@ -994,8 +1113,12 @@
       <c r="D30">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30">
+        <f t="shared" si="3"/>
+        <v>101781569</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>61</v>
       </c>
@@ -1009,8 +1132,12 @@
       <c r="D31">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31">
+        <f t="shared" si="3"/>
+        <v>100892896</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>62</v>
       </c>
@@ -1024,8 +1151,12 @@
       <c r="D32">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32">
+        <f t="shared" si="3"/>
+        <v>104924228</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>63</v>
       </c>
@@ -1039,13 +1170,17 @@
       <c r="D33">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33">
+        <f t="shared" si="3"/>
+        <v>140806276</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>64</v>
       </c>
       <c r="B34" t="str">
-        <f t="shared" ref="B34:B65" si="3">CHAR(A34)</f>
+        <f t="shared" ref="B34:B65" si="4">CHAR(A34)</f>
         <v>@</v>
       </c>
       <c r="C34">
@@ -1054,13 +1189,17 @@
       <c r="D34">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E34">
+        <f t="shared" si="3"/>
+        <v>200007183</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>65</v>
       </c>
       <c r="B35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>A</v>
       </c>
       <c r="C35">
@@ -1069,13 +1208,17 @@
       <c r="D35">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E35">
+        <f t="shared" si="3"/>
+        <v>183041585</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>66</v>
       </c>
       <c r="B36" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>B</v>
       </c>
       <c r="C36">
@@ -1084,13 +1227,17 @@
       <c r="D36">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E36">
+        <f t="shared" si="3"/>
+        <v>199817790</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>67</v>
       </c>
       <c r="B37" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>C</v>
       </c>
       <c r="C37">
@@ -1099,13 +1246,17 @@
       <c r="D37">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E37">
+        <f t="shared" si="3"/>
+        <v>141828359</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>68</v>
       </c>
       <c r="B38" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>D</v>
       </c>
       <c r="C38">
@@ -1114,13 +1265,17 @@
       <c r="D38">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E38">
+        <f t="shared" si="3"/>
+        <v>199804478</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>69</v>
       </c>
       <c r="B39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
       <c r="C39">
@@ -1129,13 +1284,17 @@
       <c r="D39">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E39">
+        <f t="shared" si="3"/>
+        <v>199782943</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>70</v>
       </c>
       <c r="B40" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>F</v>
       </c>
       <c r="C40">
@@ -1144,13 +1303,17 @@
       <c r="D40">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E40">
+        <f t="shared" si="3"/>
+        <v>150221064</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>71</v>
       </c>
       <c r="B41" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>G</v>
       </c>
       <c r="C41">
@@ -1159,13 +1322,17 @@
       <c r="D41">
         <v>5</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E41">
+        <f t="shared" si="3"/>
+        <v>183000639</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>72</v>
       </c>
       <c r="B42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>H</v>
       </c>
       <c r="C42">
@@ -1174,13 +1341,17 @@
       <c r="D42">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E42">
+        <f t="shared" si="3"/>
+        <v>143965481</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>73</v>
       </c>
       <c r="B43" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>I</v>
       </c>
       <c r="C43">
@@ -1189,13 +1360,17 @@
       <c r="D43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E43">
+        <f t="shared" si="3"/>
+        <v>34636833</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>74</v>
       </c>
       <c r="B44" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>J</v>
       </c>
       <c r="C44">
@@ -1204,13 +1379,17 @@
       <c r="D44">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E44">
+        <f t="shared" si="3"/>
+        <v>175180366</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>75</v>
       </c>
       <c r="B45" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>K</v>
       </c>
       <c r="C45">
@@ -1219,13 +1398,17 @@
       <c r="D45">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E45">
+        <f t="shared" si="3"/>
+        <v>143995209</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>76</v>
       </c>
       <c r="B46" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>L</v>
       </c>
       <c r="C46">
@@ -1234,13 +1417,17 @@
       <c r="D46">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E46">
+        <f t="shared" si="3"/>
+        <v>142876943</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>77</v>
       </c>
       <c r="B47" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>M</v>
       </c>
       <c r="C47">
@@ -1249,13 +1436,17 @@
       <c r="D47">
         <v>5</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E47">
+        <f t="shared" si="3"/>
+        <v>196794033</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>78</v>
       </c>
       <c r="B48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
       <c r="C48">
@@ -1264,13 +1455,17 @@
       <c r="D48">
         <v>5</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E48">
+        <f t="shared" si="3"/>
+        <v>186439281</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>79</v>
       </c>
       <c r="B49" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>O</v>
       </c>
       <c r="C49">
@@ -1279,13 +1474,17 @@
       <c r="D49">
         <v>5</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E49">
+        <f t="shared" si="3"/>
+        <v>183027246</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>80</v>
       </c>
       <c r="B50" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>P</v>
       </c>
       <c r="C50">
@@ -1294,13 +1493,17 @@
       <c r="D50">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E50">
+        <f t="shared" si="3"/>
+        <v>150256904</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>81</v>
       </c>
       <c r="B51" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Q</v>
       </c>
       <c r="C51">
@@ -1309,13 +1512,17 @@
       <c r="D51">
         <v>5</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E51">
+        <f t="shared" si="3"/>
+        <v>200853443</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>82</v>
       </c>
       <c r="B52" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R</v>
       </c>
       <c r="C52">
@@ -1324,13 +1531,17 @@
       <c r="D52">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E52">
+        <f t="shared" si="3"/>
+        <v>149207369</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>83</v>
       </c>
       <c r="B53" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="C53">
@@ -1339,13 +1550,17 @@
       <c r="D53">
         <v>5</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E53">
+        <f t="shared" si="3"/>
+        <v>182990894</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>84</v>
       </c>
       <c r="B54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>T</v>
       </c>
       <c r="C54">
@@ -1354,13 +1569,17 @@
       <c r="D54">
         <v>5</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E54">
+        <f t="shared" si="3"/>
+        <v>200413316</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>85</v>
       </c>
       <c r="B55" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>U</v>
       </c>
       <c r="C55">
@@ -1369,13 +1588,17 @@
       <c r="D55">
         <v>4</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E55">
+        <f t="shared" si="3"/>
+        <v>143959343</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>86</v>
       </c>
       <c r="B56" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>V</v>
       </c>
       <c r="C56">
@@ -1384,13 +1607,17 @@
       <c r="D56">
         <v>5</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E56">
+        <f t="shared" si="3"/>
+        <v>186172740</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>87</v>
       </c>
       <c r="B57" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>W</v>
       </c>
       <c r="C57">
@@ -1399,13 +1626,17 @@
       <c r="D57">
         <v>5</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E57">
+        <f t="shared" si="3"/>
+        <v>186177194</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>88</v>
       </c>
       <c r="B58" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>X</v>
       </c>
       <c r="C58">
@@ -1414,13 +1645,17 @@
       <c r="D58">
         <v>5</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E58">
+        <f t="shared" si="3"/>
+        <v>185930065</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>89</v>
       </c>
       <c r="B59" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Y</v>
       </c>
       <c r="C59">
@@ -1429,13 +1664,17 @@
       <c r="D59">
         <v>5</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E59">
+        <f t="shared" si="3"/>
+        <v>185929860</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>90</v>
       </c>
       <c r="B60" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Z</v>
       </c>
       <c r="C60">
@@ -1444,13 +1683,17 @@
       <c r="D60">
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E60">
+        <f t="shared" si="3"/>
+        <v>200347935</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>91</v>
       </c>
       <c r="B61" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>[</v>
       </c>
       <c r="C61">
@@ -1459,13 +1702,17 @@
       <c r="D61">
         <v>2</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E61">
+        <f t="shared" si="3"/>
+        <v>70322243</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>92</v>
       </c>
       <c r="B62" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>\</v>
       </c>
       <c r="C62">
@@ -1474,13 +1721,17 @@
       <c r="D62">
         <v>5</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E62">
+        <f t="shared" si="3"/>
+        <v>184815681</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>93</v>
       </c>
       <c r="B63" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>]</v>
       </c>
       <c r="C63">
@@ -1489,13 +1740,17 @@
       <c r="D63">
         <v>2</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E63">
+        <f t="shared" si="3"/>
+        <v>70288419</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>94</v>
       </c>
       <c r="B64" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>^</v>
       </c>
       <c r="C64">
@@ -1504,13 +1759,17 @@
       <c r="D64">
         <v>3</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E64">
+        <f t="shared" si="3"/>
+        <v>102924288</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>95</v>
       </c>
       <c r="B65" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>_</v>
       </c>
       <c r="C65">
@@ -1519,13 +1778,17 @@
       <c r="D65">
         <v>4</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E65">
+        <f t="shared" si="3"/>
+        <v>134217743</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>96</v>
       </c>
       <c r="B66" t="str">
-        <f t="shared" ref="B66:B97" si="4">CHAR(A66)</f>
+        <f t="shared" ref="B66:B97" si="5">CHAR(A66)</f>
         <v>`</v>
       </c>
       <c r="C66">
@@ -1534,247 +1797,511 @@
       <c r="D66">
         <v>2</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E66">
+        <f t="shared" si="3"/>
+        <v>69238784</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>97</v>
       </c>
       <c r="B67" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>a</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C67">
+        <v>199278127</v>
+      </c>
+      <c r="D67">
+        <v>5</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="3"/>
+        <v>367050287</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>98</v>
       </c>
       <c r="B68" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>b</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C68">
+        <v>185550398</v>
+      </c>
+      <c r="D68">
+        <v>5</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="3"/>
+        <v>353322558</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>99</v>
       </c>
       <c r="B69" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>c</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C69">
+        <v>183026222</v>
+      </c>
+      <c r="D69">
+        <v>5</v>
+      </c>
+      <c r="E69">
+        <f t="shared" ref="E69:E98" si="6">_xlfn.BITLSHIFT(D69,25)+C69</f>
+        <v>350798382</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>100</v>
       </c>
       <c r="B70" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>d</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C70">
+        <v>169330223</v>
+      </c>
+      <c r="D70">
+        <v>5</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="6"/>
+        <v>337102383</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>101</v>
       </c>
       <c r="B71" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>e</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C71">
+        <v>183041551</v>
+      </c>
+      <c r="D71">
+        <v>5</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="6"/>
+        <v>350813711</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>102</v>
       </c>
       <c r="B72" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>f</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C72">
+        <v>184054288</v>
+      </c>
+      <c r="D72">
+        <v>5</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="6"/>
+        <v>351826448</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>103</v>
       </c>
       <c r="B73" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>g</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C73">
+        <v>183024702</v>
+      </c>
+      <c r="D73">
+        <v>5</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="6"/>
+        <v>350796862</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>104</v>
       </c>
       <c r="B74" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>h</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C74">
+        <v>185550385</v>
+      </c>
+      <c r="D74">
+        <v>5</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="6"/>
+        <v>353322545</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>105</v>
       </c>
       <c r="B75" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>i</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C75">
+        <v>34604065</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="6"/>
+        <v>68158497</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>106</v>
       </c>
       <c r="B76" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>j</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C76">
+        <v>168854590</v>
+      </c>
+      <c r="D76">
+        <v>5</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="6"/>
+        <v>336626750</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>107</v>
       </c>
       <c r="B77" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>k</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C77">
+        <v>186217041</v>
+      </c>
+      <c r="D77">
+        <v>5</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="6"/>
+        <v>353989201</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>108</v>
       </c>
       <c r="B78" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>l</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C78">
+        <v>185090575</v>
+      </c>
+      <c r="D78">
+        <v>5</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="6"/>
+        <v>352862735</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>109</v>
       </c>
       <c r="B79" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>m</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C79">
+        <v>178968245</v>
+      </c>
+      <c r="D79">
+        <v>5</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="6"/>
+        <v>346740405</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>110</v>
       </c>
       <c r="B80" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>n</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C80">
+        <v>199804465</v>
+      </c>
+      <c r="D80">
+        <v>5</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="6"/>
+        <v>367576625</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>111</v>
       </c>
       <c r="B81" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>o</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C81">
+        <v>183027246</v>
+      </c>
+      <c r="D81">
+        <v>5</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="6"/>
+        <v>350799406</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>112</v>
       </c>
       <c r="B82" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>p</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C82">
+        <v>199804880</v>
+      </c>
+      <c r="D82">
+        <v>5</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="6"/>
+        <v>367577040</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>113</v>
       </c>
       <c r="B83" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>q</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C83">
+        <v>184075745</v>
+      </c>
+      <c r="D83">
+        <v>5</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="6"/>
+        <v>351847905</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>114</v>
       </c>
       <c r="B84" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>r</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C84">
+        <v>191676944</v>
+      </c>
+      <c r="D84">
+        <v>5</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="6"/>
+        <v>359449104</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>115</v>
       </c>
       <c r="B85" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>s</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C85">
+        <v>184039486</v>
+      </c>
+      <c r="D85">
+        <v>5</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="6"/>
+        <v>351811646</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>116</v>
       </c>
       <c r="B86" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>t</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C86">
+        <v>185483838</v>
+      </c>
+      <c r="D86">
+        <v>5</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="6"/>
+        <v>353255998</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>117</v>
       </c>
       <c r="B87" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>u</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C87">
+        <v>186173037</v>
+      </c>
+      <c r="D87">
+        <v>5</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="6"/>
+        <v>353945197</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>118</v>
       </c>
       <c r="B88" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>v</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C88">
+        <v>186165572</v>
+      </c>
+      <c r="D88">
+        <v>5</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="6"/>
+        <v>353937732</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>119</v>
       </c>
       <c r="B89" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>w</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C89">
+        <v>190502570</v>
+      </c>
+      <c r="D89">
+        <v>5</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="6"/>
+        <v>358274730</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>120</v>
       </c>
       <c r="B90" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>x</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C90">
+        <v>186169905</v>
+      </c>
+      <c r="D90">
+        <v>5</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="6"/>
+        <v>353942065</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>121</v>
       </c>
       <c r="B91" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>y</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C91">
+        <v>186170430</v>
+      </c>
+      <c r="D91">
+        <v>5</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="6"/>
+        <v>353942590</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>122</v>
       </c>
       <c r="B92" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>z</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C92">
+        <v>200347935</v>
+      </c>
+      <c r="D92">
+        <v>5</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="6"/>
+        <v>368120095</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>123</v>
       </c>
       <c r="B93" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>{</v>
       </c>
       <c r="C93">
@@ -1783,13 +2310,17 @@
       <c r="D93">
         <v>3</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E93">
+        <f t="shared" si="6"/>
+        <v>103878723</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>124</v>
       </c>
       <c r="B94" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>|</v>
       </c>
       <c r="C94">
@@ -1798,13 +2329,17 @@
       <c r="D94">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E94">
+        <f t="shared" si="6"/>
+        <v>34636833</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>125</v>
       </c>
       <c r="B95" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>}</v>
       </c>
       <c r="C95">
@@ -1813,13 +2348,17 @@
       <c r="D95">
         <v>3</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E95">
+        <f t="shared" si="6"/>
+        <v>107021382</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>126</v>
       </c>
       <c r="B96" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>~</v>
       </c>
       <c r="C96">
@@ -1828,13 +2367,17 @@
       <c r="D96">
         <v>4</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E96">
+        <f t="shared" si="6"/>
+        <v>139788288</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>127</v>
       </c>
       <c r="B97" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v></v>
       </c>
       <c r="C97">
@@ -1843,13 +2386,17 @@
       <c r="D97">
         <v>4</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E97">
+        <f t="shared" si="6"/>
+        <v>150250799</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>128</v>
       </c>
       <c r="B98" t="str">
-        <f t="shared" ref="B98:B129" si="5">CHAR(A98)</f>
+        <f t="shared" ref="B98" si="7">CHAR(A98)</f>
         <v>€</v>
       </c>
       <c r="C98">
@@ -1857,6 +2404,10 @@
       </c>
       <c r="D98">
         <v>4</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="6"/>
+        <v>150223247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add auto width finder in xlsx
</commit_message>
<xml_diff>
--- a/BigAsciiChars.xlsx
+++ b/BigAsciiChars.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30EFDB6-1255-4C3A-897F-B721AA74A978}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94E7149-BE5A-4F92-B869-F1E3BB0D5921}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18480" yWindow="4920" windowWidth="12075" windowHeight="15375" xr2:uid="{6D1A8F03-DA32-4E55-9CE4-87A60CFBC80E}"/>
+    <workbookView xWindow="3510" yWindow="1830" windowWidth="28800" windowHeight="15435" xr2:uid="{6D1A8F03-DA32-4E55-9CE4-87A60CFBC80E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Code</t>
   </si>
@@ -51,12 +51,15 @@
   <si>
     <t>FontValue</t>
   </si>
+  <si>
+    <t>&lt;== Width calculation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +73,12 @@
       <name val="Cordia New"/>
       <family val="2"/>
       <charset val="222"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -92,13 +101,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,7 +426,7 @@
   <dimension ref="A1:Q98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,7 +434,7 @@
     <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.140625" customWidth="1"/>
-    <col min="10" max="14" width="1.7109375" customWidth="1"/>
+    <col min="10" max="14" width="2.42578125" customWidth="1"/>
     <col min="16" max="16" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -457,9 +467,7 @@
       <c r="I2" s="1">
         <v>4</v>
       </c>
-      <c r="J2" s="2">
-        <v>1</v>
-      </c>
+      <c r="J2" s="2"/>
       <c r="K2" s="2">
         <v>1</v>
       </c>
@@ -469,14 +477,16 @@
       <c r="M2" s="2">
         <v>1</v>
       </c>
-      <c r="N2" s="2"/>
+      <c r="N2" s="2">
+        <v>1</v>
+      </c>
       <c r="O2">
         <f>N2+2*M2+4*L2+8*K2+16*J2</f>
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="P2">
         <f>_xlfn.BITLSHIFT(O2,5*I2)</f>
-        <v>31457280</v>
+        <v>15728640</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="17.25" x14ac:dyDescent="0.4">
@@ -504,7 +514,9 @@
         <v>3</v>
       </c>
       <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="K3" s="2">
+        <v>1</v>
+      </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2">
@@ -512,11 +524,11 @@
       </c>
       <c r="O3">
         <f t="shared" ref="O3:O6" si="1">N3+2*M3+4*L3+8*K3+16*J3</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="P3">
         <f t="shared" ref="P3:P6" si="2">_xlfn.BITLSHIFT(O3,5*I3)</f>
-        <v>32768</v>
+        <v>294912</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="17.25" x14ac:dyDescent="0.4">
@@ -587,22 +599,20 @@
       <c r="I5" s="1">
         <v>1</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="2"/>
+      <c r="K5" s="2">
         <v>1</v>
       </c>
-      <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
-      <c r="N5" s="2">
-        <v>1</v>
-      </c>
+      <c r="N5" s="2"/>
       <c r="O5">
         <f>N5+2*M5+4*L5+8*K5+16*J5</f>
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="P5">
         <f t="shared" si="2"/>
-        <v>544</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
@@ -631,22 +641,16 @@
       <c r="K6" s="2">
         <v>1</v>
       </c>
-      <c r="L6" s="2">
-        <v>1</v>
-      </c>
-      <c r="M6" s="2">
-        <v>1</v>
-      </c>
-      <c r="N6" s="2">
-        <v>1</v>
-      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
       <c r="O6">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="P6">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -668,8 +672,8 @@
         <v>194842995</v>
       </c>
       <c r="P7">
-        <f>SUM(P2:P6)</f>
-        <v>31505967</v>
+        <f>SUM(P2:P6)+P9</f>
+        <v>150256904</v>
       </c>
       <c r="Q7" t="s">
         <v>6</v>
@@ -713,6 +717,37 @@
         <f t="shared" si="3"/>
         <v>68222976</v>
       </c>
+      <c r="J9" s="4">
+        <f>MAX(J2:J6)</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
+        <f t="shared" ref="K9:N9" si="4">MAX(K2:K6)</f>
+        <v>1</v>
+      </c>
+      <c r="L9" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M9" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N9" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O9" s="4">
+        <f>6-MATCH(1,J9:N9,0)</f>
+        <v>4</v>
+      </c>
+      <c r="P9" s="4">
+        <f>_xlfn.BITLSHIFT(O9,25)</f>
+        <v>134217728</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1175,7 +1210,7 @@
         <v>64</v>
       </c>
       <c r="B34" t="str">
-        <f t="shared" ref="B34:B65" si="4">CHAR(A34)</f>
+        <f t="shared" ref="B34:B65" si="5">CHAR(A34)</f>
         <v>@</v>
       </c>
       <c r="C34">
@@ -1194,7 +1229,7 @@
         <v>65</v>
       </c>
       <c r="B35" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>A</v>
       </c>
       <c r="C35">
@@ -1213,7 +1248,7 @@
         <v>66</v>
       </c>
       <c r="B36" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>B</v>
       </c>
       <c r="C36">
@@ -1232,7 +1267,7 @@
         <v>67</v>
       </c>
       <c r="B37" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>C</v>
       </c>
       <c r="C37">
@@ -1251,7 +1286,7 @@
         <v>68</v>
       </c>
       <c r="B38" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>D</v>
       </c>
       <c r="C38">
@@ -1270,7 +1305,7 @@
         <v>69</v>
       </c>
       <c r="B39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E</v>
       </c>
       <c r="C39">
@@ -1289,7 +1324,7 @@
         <v>70</v>
       </c>
       <c r="B40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>F</v>
       </c>
       <c r="C40">
@@ -1308,7 +1343,7 @@
         <v>71</v>
       </c>
       <c r="B41" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>G</v>
       </c>
       <c r="C41">
@@ -1327,7 +1362,7 @@
         <v>72</v>
       </c>
       <c r="B42" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>H</v>
       </c>
       <c r="C42">
@@ -1346,7 +1381,7 @@
         <v>73</v>
       </c>
       <c r="B43" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>I</v>
       </c>
       <c r="C43">
@@ -1365,7 +1400,7 @@
         <v>74</v>
       </c>
       <c r="B44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>J</v>
       </c>
       <c r="C44">
@@ -1384,7 +1419,7 @@
         <v>75</v>
       </c>
       <c r="B45" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>K</v>
       </c>
       <c r="C45">
@@ -1403,7 +1438,7 @@
         <v>76</v>
       </c>
       <c r="B46" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>L</v>
       </c>
       <c r="C46">
@@ -1422,7 +1457,7 @@
         <v>77</v>
       </c>
       <c r="B47" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>M</v>
       </c>
       <c r="C47">
@@ -1441,7 +1476,7 @@
         <v>78</v>
       </c>
       <c r="B48" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>N</v>
       </c>
       <c r="C48">
@@ -1460,7 +1495,7 @@
         <v>79</v>
       </c>
       <c r="B49" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>O</v>
       </c>
       <c r="C49">
@@ -1479,7 +1514,7 @@
         <v>80</v>
       </c>
       <c r="B50" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>P</v>
       </c>
       <c r="C50">
@@ -1498,7 +1533,7 @@
         <v>81</v>
       </c>
       <c r="B51" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Q</v>
       </c>
       <c r="C51">
@@ -1517,7 +1552,7 @@
         <v>82</v>
       </c>
       <c r="B52" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>R</v>
       </c>
       <c r="C52">
@@ -1536,7 +1571,7 @@
         <v>83</v>
       </c>
       <c r="B53" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="C53">
@@ -1555,7 +1590,7 @@
         <v>84</v>
       </c>
       <c r="B54" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>T</v>
       </c>
       <c r="C54">
@@ -1574,7 +1609,7 @@
         <v>85</v>
       </c>
       <c r="B55" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>U</v>
       </c>
       <c r="C55">
@@ -1593,7 +1628,7 @@
         <v>86</v>
       </c>
       <c r="B56" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>V</v>
       </c>
       <c r="C56">
@@ -1612,7 +1647,7 @@
         <v>87</v>
       </c>
       <c r="B57" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>W</v>
       </c>
       <c r="C57">
@@ -1631,7 +1666,7 @@
         <v>88</v>
       </c>
       <c r="B58" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>X</v>
       </c>
       <c r="C58">
@@ -1650,7 +1685,7 @@
         <v>89</v>
       </c>
       <c r="B59" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Y</v>
       </c>
       <c r="C59">
@@ -1669,7 +1704,7 @@
         <v>90</v>
       </c>
       <c r="B60" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Z</v>
       </c>
       <c r="C60">
@@ -1688,7 +1723,7 @@
         <v>91</v>
       </c>
       <c r="B61" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>[</v>
       </c>
       <c r="C61">
@@ -1707,7 +1742,7 @@
         <v>92</v>
       </c>
       <c r="B62" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>\</v>
       </c>
       <c r="C62">
@@ -1726,7 +1761,7 @@
         <v>93</v>
       </c>
       <c r="B63" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>]</v>
       </c>
       <c r="C63">
@@ -1745,7 +1780,7 @@
         <v>94</v>
       </c>
       <c r="B64" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>^</v>
       </c>
       <c r="C64">
@@ -1764,7 +1799,7 @@
         <v>95</v>
       </c>
       <c r="B65" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>_</v>
       </c>
       <c r="C65">
@@ -1783,7 +1818,7 @@
         <v>96</v>
       </c>
       <c r="B66" t="str">
-        <f t="shared" ref="B66:B97" si="5">CHAR(A66)</f>
+        <f t="shared" ref="B66:B97" si="6">CHAR(A66)</f>
         <v>`</v>
       </c>
       <c r="C66">
@@ -1802,7 +1837,7 @@
         <v>97</v>
       </c>
       <c r="B67" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>a</v>
       </c>
       <c r="C67">
@@ -1821,7 +1856,7 @@
         <v>98</v>
       </c>
       <c r="B68" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>b</v>
       </c>
       <c r="C68">
@@ -1840,7 +1875,7 @@
         <v>99</v>
       </c>
       <c r="B69" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>c</v>
       </c>
       <c r="C69">
@@ -1850,7 +1885,7 @@
         <v>5</v>
       </c>
       <c r="E69">
-        <f t="shared" ref="E69:E98" si="6">_xlfn.BITLSHIFT(D69,25)+C69</f>
+        <f t="shared" ref="E69:E98" si="7">_xlfn.BITLSHIFT(D69,25)+C69</f>
         <v>350798382</v>
       </c>
     </row>
@@ -1859,7 +1894,7 @@
         <v>100</v>
       </c>
       <c r="B70" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>d</v>
       </c>
       <c r="C70">
@@ -1869,7 +1904,7 @@
         <v>5</v>
       </c>
       <c r="E70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>337102383</v>
       </c>
     </row>
@@ -1878,7 +1913,7 @@
         <v>101</v>
       </c>
       <c r="B71" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>e</v>
       </c>
       <c r="C71">
@@ -1888,7 +1923,7 @@
         <v>5</v>
       </c>
       <c r="E71">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>350813711</v>
       </c>
     </row>
@@ -1897,7 +1932,7 @@
         <v>102</v>
       </c>
       <c r="B72" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>f</v>
       </c>
       <c r="C72">
@@ -1907,7 +1942,7 @@
         <v>5</v>
       </c>
       <c r="E72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>351826448</v>
       </c>
     </row>
@@ -1916,7 +1951,7 @@
         <v>103</v>
       </c>
       <c r="B73" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>g</v>
       </c>
       <c r="C73">
@@ -1926,7 +1961,7 @@
         <v>5</v>
       </c>
       <c r="E73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>350796862</v>
       </c>
     </row>
@@ -1935,7 +1970,7 @@
         <v>104</v>
       </c>
       <c r="B74" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>h</v>
       </c>
       <c r="C74">
@@ -1945,7 +1980,7 @@
         <v>5</v>
       </c>
       <c r="E74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>353322545</v>
       </c>
     </row>
@@ -1954,7 +1989,7 @@
         <v>105</v>
       </c>
       <c r="B75" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>i</v>
       </c>
       <c r="C75">
@@ -1964,7 +1999,7 @@
         <v>1</v>
       </c>
       <c r="E75">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>68158497</v>
       </c>
     </row>
@@ -1973,7 +2008,7 @@
         <v>106</v>
       </c>
       <c r="B76" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>j</v>
       </c>
       <c r="C76">
@@ -1983,7 +2018,7 @@
         <v>5</v>
       </c>
       <c r="E76">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>336626750</v>
       </c>
     </row>
@@ -1992,7 +2027,7 @@
         <v>107</v>
       </c>
       <c r="B77" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>k</v>
       </c>
       <c r="C77">
@@ -2002,7 +2037,7 @@
         <v>5</v>
       </c>
       <c r="E77">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>353989201</v>
       </c>
     </row>
@@ -2011,7 +2046,7 @@
         <v>108</v>
       </c>
       <c r="B78" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>l</v>
       </c>
       <c r="C78">
@@ -2021,7 +2056,7 @@
         <v>5</v>
       </c>
       <c r="E78">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>352862735</v>
       </c>
     </row>
@@ -2030,7 +2065,7 @@
         <v>109</v>
       </c>
       <c r="B79" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>m</v>
       </c>
       <c r="C79">
@@ -2040,7 +2075,7 @@
         <v>5</v>
       </c>
       <c r="E79">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>346740405</v>
       </c>
     </row>
@@ -2049,7 +2084,7 @@
         <v>110</v>
       </c>
       <c r="B80" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>n</v>
       </c>
       <c r="C80">
@@ -2059,7 +2094,7 @@
         <v>5</v>
       </c>
       <c r="E80">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>367576625</v>
       </c>
     </row>
@@ -2068,7 +2103,7 @@
         <v>111</v>
       </c>
       <c r="B81" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>o</v>
       </c>
       <c r="C81">
@@ -2078,7 +2113,7 @@
         <v>5</v>
       </c>
       <c r="E81">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>350799406</v>
       </c>
     </row>
@@ -2087,7 +2122,7 @@
         <v>112</v>
       </c>
       <c r="B82" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>p</v>
       </c>
       <c r="C82">
@@ -2097,7 +2132,7 @@
         <v>5</v>
       </c>
       <c r="E82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>367577040</v>
       </c>
     </row>
@@ -2106,7 +2141,7 @@
         <v>113</v>
       </c>
       <c r="B83" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>q</v>
       </c>
       <c r="C83">
@@ -2116,7 +2151,7 @@
         <v>5</v>
       </c>
       <c r="E83">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>351847905</v>
       </c>
     </row>
@@ -2125,7 +2160,7 @@
         <v>114</v>
       </c>
       <c r="B84" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>r</v>
       </c>
       <c r="C84">
@@ -2135,7 +2170,7 @@
         <v>5</v>
       </c>
       <c r="E84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>359449104</v>
       </c>
     </row>
@@ -2144,7 +2179,7 @@
         <v>115</v>
       </c>
       <c r="B85" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>s</v>
       </c>
       <c r="C85">
@@ -2154,7 +2189,7 @@
         <v>5</v>
       </c>
       <c r="E85">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>351811646</v>
       </c>
     </row>
@@ -2163,7 +2198,7 @@
         <v>116</v>
       </c>
       <c r="B86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>t</v>
       </c>
       <c r="C86">
@@ -2173,7 +2208,7 @@
         <v>5</v>
       </c>
       <c r="E86">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>353255998</v>
       </c>
     </row>
@@ -2182,7 +2217,7 @@
         <v>117</v>
       </c>
       <c r="B87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>u</v>
       </c>
       <c r="C87">
@@ -2192,7 +2227,7 @@
         <v>5</v>
       </c>
       <c r="E87">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>353945197</v>
       </c>
     </row>
@@ -2201,7 +2236,7 @@
         <v>118</v>
       </c>
       <c r="B88" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>v</v>
       </c>
       <c r="C88">
@@ -2211,7 +2246,7 @@
         <v>5</v>
       </c>
       <c r="E88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>353937732</v>
       </c>
     </row>
@@ -2220,7 +2255,7 @@
         <v>119</v>
       </c>
       <c r="B89" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>w</v>
       </c>
       <c r="C89">
@@ -2230,7 +2265,7 @@
         <v>5</v>
       </c>
       <c r="E89">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>358274730</v>
       </c>
     </row>
@@ -2239,7 +2274,7 @@
         <v>120</v>
       </c>
       <c r="B90" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>x</v>
       </c>
       <c r="C90">
@@ -2249,7 +2284,7 @@
         <v>5</v>
       </c>
       <c r="E90">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>353942065</v>
       </c>
     </row>
@@ -2258,7 +2293,7 @@
         <v>121</v>
       </c>
       <c r="B91" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>y</v>
       </c>
       <c r="C91">
@@ -2268,7 +2303,7 @@
         <v>5</v>
       </c>
       <c r="E91">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>353942590</v>
       </c>
     </row>
@@ -2277,7 +2312,7 @@
         <v>122</v>
       </c>
       <c r="B92" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>z</v>
       </c>
       <c r="C92">
@@ -2287,7 +2322,7 @@
         <v>5</v>
       </c>
       <c r="E92">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>368120095</v>
       </c>
     </row>
@@ -2296,7 +2331,7 @@
         <v>123</v>
       </c>
       <c r="B93" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>{</v>
       </c>
       <c r="C93">
@@ -2306,7 +2341,7 @@
         <v>3</v>
       </c>
       <c r="E93">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>103878723</v>
       </c>
     </row>
@@ -2315,7 +2350,7 @@
         <v>124</v>
       </c>
       <c r="B94" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>|</v>
       </c>
       <c r="C94">
@@ -2325,7 +2360,7 @@
         <v>1</v>
       </c>
       <c r="E94">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>34636833</v>
       </c>
     </row>
@@ -2334,7 +2369,7 @@
         <v>125</v>
       </c>
       <c r="B95" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>}</v>
       </c>
       <c r="C95">
@@ -2344,7 +2379,7 @@
         <v>3</v>
       </c>
       <c r="E95">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>107021382</v>
       </c>
     </row>
@@ -2353,7 +2388,7 @@
         <v>126</v>
       </c>
       <c r="B96" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>~</v>
       </c>
       <c r="C96">
@@ -2363,7 +2398,7 @@
         <v>4</v>
       </c>
       <c r="E96">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>139788288</v>
       </c>
     </row>
@@ -2372,7 +2407,7 @@
         <v>127</v>
       </c>
       <c r="B97" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v></v>
       </c>
       <c r="C97">
@@ -2382,7 +2417,7 @@
         <v>4</v>
       </c>
       <c r="E97">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>150250799</v>
       </c>
     </row>
@@ -2391,7 +2426,7 @@
         <v>128</v>
       </c>
       <c r="B98" t="str">
-        <f t="shared" ref="B98" si="7">CHAR(A98)</f>
+        <f t="shared" ref="B98" si="8">CHAR(A98)</f>
         <v>€</v>
       </c>
       <c r="C98">
@@ -2401,7 +2436,7 @@
         <v>4</v>
       </c>
       <c r="E98">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>150223247</v>
       </c>
     </row>

</xml_diff>

<commit_message>
WIP of conversion to class based font
</commit_message>
<xml_diff>
--- a/BigAsciiChars.xlsx
+++ b/BigAsciiChars.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94E7149-BE5A-4F92-B869-F1E3BB0D5921}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDE2B74-7B29-470F-B849-50F646031769}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="1830" windowWidth="28800" windowHeight="15435" xr2:uid="{6D1A8F03-DA32-4E55-9CE4-87A60CFBC80E}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="27634" windowHeight="14417" xr2:uid="{6D1A8F03-DA32-4E55-9CE4-87A60CFBC80E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="5x5" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -426,19 +426,19 @@
   <dimension ref="A1:Q98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+      <selection activeCell="P6" sqref="P2:P6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" customWidth="1"/>
-    <col min="10" max="14" width="2.42578125" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.84375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.84375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.15234375" customWidth="1"/>
+    <col min="10" max="14" width="2.3828125" customWidth="1"/>
+    <col min="16" max="16" width="12.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,7 +455,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>32</v>
       </c>
@@ -489,7 +489,7 @@
         <v>15728640</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="17.25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:17" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>33</v>
       </c>
@@ -531,7 +531,7 @@
         <v>294912</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="17.25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:17" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>34</v>
       </c>
@@ -559,25 +559,21 @@
       <c r="K4" s="2">
         <v>1</v>
       </c>
-      <c r="L4" s="2">
-        <v>1</v>
-      </c>
-      <c r="M4" s="2">
-        <v>1</v>
-      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
       <c r="N4" s="2">
         <v>1</v>
       </c>
       <c r="O4">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="P4">
         <f t="shared" si="2"/>
-        <v>15360</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
+        <v>9216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>35</v>
       </c>
@@ -605,17 +601,19 @@
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
+      <c r="N5" s="2">
+        <v>1</v>
+      </c>
       <c r="O5">
         <f>N5+2*M5+4*L5+8*K5+16*J5</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="P5">
         <f t="shared" si="2"/>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>36</v>
       </c>
@@ -641,19 +639,25 @@
       <c r="K6" s="2">
         <v>1</v>
       </c>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
+      <c r="L6" s="2">
+        <v>1</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1</v>
+      </c>
+      <c r="N6" s="2">
+        <v>1</v>
+      </c>
       <c r="O6">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="P6">
         <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>37</v>
       </c>
@@ -673,13 +677,13 @@
       </c>
       <c r="P7">
         <f>SUM(P2:P6)+P9</f>
-        <v>150256904</v>
+        <v>150250799</v>
       </c>
       <c r="Q7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>38</v>
       </c>
@@ -699,7 +703,7 @@
       </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>39</v>
       </c>
@@ -749,7 +753,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>40</v>
       </c>
@@ -768,7 +772,7 @@
         <v>68225089</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>41</v>
       </c>
@@ -787,7 +791,7 @@
         <v>69239842</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>42</v>
       </c>
@@ -806,7 +810,7 @@
         <v>185750673</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>43</v>
       </c>
@@ -825,7 +829,7 @@
         <v>172129412</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>44</v>
       </c>
@@ -844,7 +848,7 @@
         <v>67108898</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>45</v>
       </c>
@@ -863,7 +867,7 @@
         <v>100670464</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>46</v>
       </c>
@@ -882,7 +886,7 @@
         <v>67108963</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>47</v>
       </c>
@@ -901,7 +905,7 @@
         <v>168890640</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>48</v>
       </c>
@@ -920,7 +924,7 @@
         <v>140813606</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>49</v>
       </c>
@@ -939,7 +943,7 @@
         <v>107022407</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>50</v>
       </c>
@@ -958,7 +962,7 @@
         <v>140806287</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>51</v>
       </c>
@@ -977,7 +981,7 @@
         <v>183015982</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>52</v>
       </c>
@@ -996,7 +1000,7 @@
         <v>142949442</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>53</v>
       </c>
@@ -1015,7 +1019,7 @@
         <v>150222894</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>54</v>
       </c>
@@ -1034,7 +1038,7 @@
         <v>141834534</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>55</v>
       </c>
@@ -1053,7 +1057,7 @@
         <v>150016264</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>56</v>
       </c>
@@ -1072,7 +1076,7 @@
         <v>140810534</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>57</v>
       </c>
@@ -1091,7 +1095,7 @@
         <v>140811302</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>58</v>
       </c>
@@ -1110,7 +1114,7 @@
         <v>33587201</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>59</v>
       </c>
@@ -1129,7 +1133,7 @@
         <v>67141666</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>60</v>
       </c>
@@ -1148,7 +1152,7 @@
         <v>101781569</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>61</v>
       </c>
@@ -1167,7 +1171,7 @@
         <v>100892896</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>62</v>
       </c>
@@ -1186,7 +1190,7 @@
         <v>104924228</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>63</v>
       </c>
@@ -1205,7 +1209,7 @@
         <v>140806276</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>64</v>
       </c>
@@ -1224,7 +1228,7 @@
         <v>200007183</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>65</v>
       </c>
@@ -1243,7 +1247,7 @@
         <v>183041585</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>66</v>
       </c>
@@ -1262,7 +1266,7 @@
         <v>199817790</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>67</v>
       </c>
@@ -1281,7 +1285,7 @@
         <v>141828359</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>68</v>
       </c>
@@ -1300,7 +1304,7 @@
         <v>199804478</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>69</v>
       </c>
@@ -1319,7 +1323,7 @@
         <v>199782943</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>70</v>
       </c>
@@ -1338,7 +1342,7 @@
         <v>150221064</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>71</v>
       </c>
@@ -1357,7 +1361,7 @@
         <v>183000639</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>72</v>
       </c>
@@ -1376,7 +1380,7 @@
         <v>143965481</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>73</v>
       </c>
@@ -1395,7 +1399,7 @@
         <v>34636833</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>74</v>
       </c>
@@ -1414,7 +1418,7 @@
         <v>175180366</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>75</v>
       </c>
@@ -1433,7 +1437,7 @@
         <v>143995209</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>76</v>
       </c>
@@ -1452,7 +1456,7 @@
         <v>142876943</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>77</v>
       </c>
@@ -1471,7 +1475,7 @@
         <v>196794033</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>78</v>
       </c>
@@ -1490,7 +1494,7 @@
         <v>186439281</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>79</v>
       </c>
@@ -1509,7 +1513,7 @@
         <v>183027246</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>80</v>
       </c>
@@ -1528,7 +1532,7 @@
         <v>150256904</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>81</v>
       </c>
@@ -1547,7 +1551,7 @@
         <v>200853443</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>82</v>
       </c>
@@ -1566,7 +1570,7 @@
         <v>149207369</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>83</v>
       </c>
@@ -1585,7 +1589,7 @@
         <v>182990894</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>84</v>
       </c>
@@ -1604,7 +1608,7 @@
         <v>200413316</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A55">
         <v>85</v>
       </c>
@@ -1623,7 +1627,7 @@
         <v>143959343</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A56">
         <v>86</v>
       </c>
@@ -1642,7 +1646,7 @@
         <v>186172740</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A57">
         <v>87</v>
       </c>
@@ -1661,7 +1665,7 @@
         <v>186177194</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A58">
         <v>88</v>
       </c>
@@ -1680,7 +1684,7 @@
         <v>185930065</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A59">
         <v>89</v>
       </c>
@@ -1699,7 +1703,7 @@
         <v>185929860</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A60">
         <v>90</v>
       </c>
@@ -1718,7 +1722,7 @@
         <v>200347935</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A61">
         <v>91</v>
       </c>
@@ -1737,7 +1741,7 @@
         <v>70322243</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A62">
         <v>92</v>
       </c>
@@ -1756,7 +1760,7 @@
         <v>184815681</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A63">
         <v>93</v>
       </c>
@@ -1775,7 +1779,7 @@
         <v>70288419</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A64">
         <v>94</v>
       </c>
@@ -1794,7 +1798,7 @@
         <v>102924288</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A65">
         <v>95</v>
       </c>
@@ -1813,7 +1817,7 @@
         <v>134217743</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A66">
         <v>96</v>
       </c>
@@ -1832,7 +1836,7 @@
         <v>69238784</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A67">
         <v>97</v>
       </c>
@@ -1851,7 +1855,7 @@
         <v>367050287</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A68">
         <v>98</v>
       </c>
@@ -1870,7 +1874,7 @@
         <v>353322558</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A69">
         <v>99</v>
       </c>
@@ -1889,7 +1893,7 @@
         <v>350798382</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A70">
         <v>100</v>
       </c>
@@ -1908,7 +1912,7 @@
         <v>337102383</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A71">
         <v>101</v>
       </c>
@@ -1927,7 +1931,7 @@
         <v>350813711</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A72">
         <v>102</v>
       </c>
@@ -1946,7 +1950,7 @@
         <v>351826448</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A73">
         <v>103</v>
       </c>
@@ -1965,7 +1969,7 @@
         <v>350796862</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A74">
         <v>104</v>
       </c>
@@ -1984,7 +1988,7 @@
         <v>353322545</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A75">
         <v>105</v>
       </c>
@@ -2003,7 +2007,7 @@
         <v>68158497</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A76">
         <v>106</v>
       </c>
@@ -2022,7 +2026,7 @@
         <v>336626750</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A77">
         <v>107</v>
       </c>
@@ -2041,7 +2045,7 @@
         <v>353989201</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A78">
         <v>108</v>
       </c>
@@ -2060,7 +2064,7 @@
         <v>352862735</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A79">
         <v>109</v>
       </c>
@@ -2079,7 +2083,7 @@
         <v>346740405</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A80">
         <v>110</v>
       </c>
@@ -2098,7 +2102,7 @@
         <v>367576625</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A81">
         <v>111</v>
       </c>
@@ -2117,7 +2121,7 @@
         <v>350799406</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A82">
         <v>112</v>
       </c>
@@ -2136,7 +2140,7 @@
         <v>367577040</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A83">
         <v>113</v>
       </c>
@@ -2155,7 +2159,7 @@
         <v>351847905</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A84">
         <v>114</v>
       </c>
@@ -2174,7 +2178,7 @@
         <v>359449104</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A85">
         <v>115</v>
       </c>
@@ -2193,7 +2197,7 @@
         <v>351811646</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A86">
         <v>116</v>
       </c>
@@ -2212,7 +2216,7 @@
         <v>353255998</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A87">
         <v>117</v>
       </c>
@@ -2231,7 +2235,7 @@
         <v>353945197</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A88">
         <v>118</v>
       </c>
@@ -2250,7 +2254,7 @@
         <v>353937732</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A89">
         <v>119</v>
       </c>
@@ -2269,7 +2273,7 @@
         <v>358274730</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A90">
         <v>120</v>
       </c>
@@ -2288,7 +2292,7 @@
         <v>353942065</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A91">
         <v>121</v>
       </c>
@@ -2307,7 +2311,7 @@
         <v>353942590</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A92">
         <v>122</v>
       </c>
@@ -2326,7 +2330,7 @@
         <v>368120095</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A93">
         <v>123</v>
       </c>
@@ -2345,7 +2349,7 @@
         <v>103878723</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A94">
         <v>124</v>
       </c>
@@ -2364,7 +2368,7 @@
         <v>34636833</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A95">
         <v>125</v>
       </c>
@@ -2383,7 +2387,7 @@
         <v>107021382</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A96">
         <v>126</v>
       </c>
@@ -2402,7 +2406,7 @@
         <v>139788288</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A97">
         <v>127</v>
       </c>
@@ -2421,7 +2425,7 @@
         <v>150250799</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A98">
         <v>128</v>
       </c>

</xml_diff>

<commit_message>
Update xlsx with 8x8 values (wip) and whitespace tweaks
</commit_message>
<xml_diff>
--- a/BigAsciiChars.xlsx
+++ b/BigAsciiChars.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1396DF-A64E-4FE1-A191-3723E0456AC9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD675179-7F2A-4540-81A3-9EFE64230C68}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6555" yWindow="3495" windowWidth="23250" windowHeight="13485" activeTab="2" xr2:uid="{6D1A8F03-DA32-4E55-9CE4-87A60CFBC80E}"/>
+    <workbookView xWindow="1695" yWindow="60" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{6D1A8F03-DA32-4E55-9CE4-87A60CFBC80E}"/>
   </bookViews>
   <sheets>
     <sheet name="5x5" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="131">
   <si>
     <t>Code</t>
   </si>
@@ -60,9 +60,6 @@
     <t xml:space="preserve">Width = </t>
   </si>
   <si>
-    <t xml:space="preserve"># </t>
-  </si>
-  <si>
     <t>=</t>
   </si>
   <si>
@@ -75,10 +72,355 @@
     <t>This is your value to use ==&gt;</t>
   </si>
   <si>
-    <t>0x040A001E213E201E</t>
-  </si>
-  <si>
     <t>Put a character in each cell</t>
+  </si>
+  <si>
+    <t>0x0814001E213E201E</t>
+  </si>
+  <si>
+    <t>0x0000001E213E201E</t>
+  </si>
+  <si>
+    <t>0x0408101E213E201E</t>
+  </si>
+  <si>
+    <t>0x1008041E213E201E</t>
+  </si>
+  <si>
+    <t>0x0014001E213E201E</t>
+  </si>
+  <si>
+    <t>0x0005000202020202</t>
+  </si>
+  <si>
+    <t>0x0205000202020202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   # </t>
+  </si>
+  <si>
+    <t>0x0201000101010101</t>
+  </si>
+  <si>
+    <t>0x0102000202020202</t>
+  </si>
+  <si>
+    <t>0x0000020002020202</t>
+  </si>
+  <si>
+    <t>0x0A14002C32222222</t>
+  </si>
+  <si>
+    <t>0x1619111111</t>
+  </si>
+  <si>
+    <t>0x000A0C020911110E</t>
+  </si>
+  <si>
+    <t>0x0804001E2121211E</t>
+  </si>
+  <si>
+    <t>0x0408001E2121211E</t>
+  </si>
+  <si>
+    <t>0x0814001E2121211E</t>
+  </si>
+  <si>
+    <t>0x0A14001E2121211E</t>
+  </si>
+  <si>
+    <t>0x0012001E2121211E</t>
+  </si>
+  <si>
+    <t>0x0000001E2121211E</t>
+  </si>
+  <si>
+    <t>0x000008007F000800</t>
+  </si>
+  <si>
+    <t>0x00011E2529313E40</t>
+  </si>
+  <si>
+    <t>0x000804111111110E</t>
+  </si>
+  <si>
+    <t>0x000204111111110E</t>
+  </si>
+  <si>
+    <t>0x040A00111111110E</t>
+  </si>
+  <si>
+    <t>0x000A00111111110E</t>
+  </si>
+  <si>
+    <t>0x000000111111110E</t>
+  </si>
+  <si>
+    <t>0x000204110A040810</t>
+  </si>
+  <si>
+    <t>0x0010141A11111A14</t>
+  </si>
+  <si>
+    <t>0x000A00110A040810</t>
+  </si>
+  <si>
+    <t>0x000E1110110E0418</t>
+  </si>
+  <si>
+    <t>0x000076093F484936</t>
+  </si>
+  <si>
+    <t>0x0814081E2222221D</t>
+  </si>
+  <si>
+    <t>0x0014001E2222221D</t>
+  </si>
+  <si>
+    <t>0x0A14001E2222221D</t>
+  </si>
+  <si>
+    <t>0x0814001E2222221D</t>
+  </si>
+  <si>
+    <t>0x0804001E2222221D</t>
+  </si>
+  <si>
+    <t>0x0408001E2222221D</t>
+  </si>
+  <si>
+    <t>0x407C424141427C40</t>
+  </si>
+  <si>
+    <t>0x1C2222242C22212E</t>
+  </si>
+  <si>
+    <t>0x0851221408080808</t>
+  </si>
+  <si>
+    <t>0x081441414141413E</t>
+  </si>
+  <si>
+    <t>0x140041414141413E</t>
+  </si>
+  <si>
+    <t>0x040841414141413E</t>
+  </si>
+  <si>
+    <t>0x100841414141413E</t>
+  </si>
+  <si>
+    <t>0x14003E414141413E</t>
+  </si>
+  <si>
+    <t>0x0A143E414141413E</t>
+  </si>
+  <si>
+    <t>0x08143E414141413E</t>
+  </si>
+  <si>
+    <t>0x08103E414141413E</t>
+  </si>
+  <si>
+    <t>0x08043E414141413E</t>
+  </si>
+  <si>
+    <t>0x110A040A1100</t>
+  </si>
+  <si>
+    <t>0x013E464A52627C80</t>
+  </si>
+  <si>
+    <t>0xA14213129252321</t>
+  </si>
+  <si>
+    <t>0x3C22217921223C</t>
+  </si>
+  <si>
+    <t>0x0500020202020202</t>
+  </si>
+  <si>
+    <t>0x0205020202020202</t>
+  </si>
+  <si>
+    <t>0x0102010101010101</t>
+  </si>
+  <si>
+    <t>0x0201020202020202</t>
+  </si>
+  <si>
+    <t>0x12003F203E20203F</t>
+  </si>
+  <si>
+    <t>0x08143F203E20203F</t>
+  </si>
+  <si>
+    <t>0x04083F203E20203F</t>
+  </si>
+  <si>
+    <t>0x08043F203E20203F</t>
+  </si>
+  <si>
+    <t>0x1F202020201F040C</t>
+  </si>
+  <si>
+    <t>0x1F284888FF88888F</t>
+  </si>
+  <si>
+    <t>0x08140808143E4141</t>
+  </si>
+  <si>
+    <t>0x14001C22417F4141</t>
+  </si>
+  <si>
+    <t>0x14283C4281FF8181</t>
+  </si>
+  <si>
+    <t>0x08141C22417F4141</t>
+  </si>
+  <si>
+    <t>0x04081C22417F4141</t>
+  </si>
+  <si>
+    <t>0x08041C22417F4141</t>
+  </si>
+  <si>
+    <t>0x040004081010110E</t>
+  </si>
+  <si>
+    <t>0x2022240A142B0200</t>
+  </si>
+  <si>
+    <t>0x2022240A15220700</t>
+  </si>
+  <si>
+    <t>0xC022E42AD4274202</t>
+  </si>
+  <si>
+    <t>0x0028140A050A1428</t>
+  </si>
+  <si>
+    <t>0x1C2222221C003E00</t>
+  </si>
+  <si>
+    <t>0x0103010101000000</t>
+  </si>
+  <si>
+    <t>0x000000000000040C</t>
+  </si>
+  <si>
+    <t>0x0000000006060000</t>
+  </si>
+  <si>
+    <t>0x001F393919090909</t>
+  </si>
+  <si>
+    <t>0x00002222221E2120</t>
+  </si>
+  <si>
+    <t>0x0102000000000000</t>
+  </si>
+  <si>
+    <t>0x0601060106000000</t>
+  </si>
+  <si>
+    <t>0x0205010207000000</t>
+  </si>
+  <si>
+    <t>0x04041F0404001F00</t>
+  </si>
+  <si>
+    <t>0x0205020000000000</t>
+  </si>
+  <si>
+    <t>0x0007000000000000</t>
+  </si>
+  <si>
+    <t>0x3E4D5151513E0000</t>
+  </si>
+  <si>
+    <t>0x0000001F00000000</t>
+  </si>
+  <si>
+    <t>0x00003F0100000000</t>
+  </si>
+  <si>
+    <t>0x00050A1428140A05</t>
+  </si>
+  <si>
+    <t>0x06010F090F001F00</t>
+  </si>
+  <si>
+    <t>0x7E81BDA1A1BD817E</t>
+  </si>
+  <si>
+    <t>0x0024000000000000</t>
+  </si>
+  <si>
+    <t>0x3C403C24243C023C</t>
+  </si>
+  <si>
+    <t>0x0101010000010101</t>
+  </si>
+  <si>
+    <t>0x412214087F087F08</t>
+  </si>
+  <si>
+    <t>0x110E1111110E11</t>
+  </si>
+  <si>
+    <t>0x001E20207C20207F</t>
+  </si>
+  <si>
+    <t>0x041E212020211E04</t>
+  </si>
+  <si>
+    <t>0x0100010101010101</t>
+  </si>
+  <si>
+    <t>0x1441221408080808</t>
+  </si>
+  <si>
+    <t>0x0A04001F0204081F</t>
+  </si>
+  <si>
+    <t>0x00000077898F8877</t>
+  </si>
+  <si>
+    <t>0x007F88888F88887F</t>
+  </si>
+  <si>
+    <t>0x0008040201020408</t>
+  </si>
+  <si>
+    <t>0x050200070802010E</t>
+  </si>
+  <si>
+    <t>0xEA55550000000000</t>
+  </si>
+  <si>
+    <t>0x1926000000000000</t>
+  </si>
+  <si>
+    <t>0x00000000FF000000</t>
+  </si>
+  <si>
+    <t>0x000000003F000000</t>
+  </si>
+  <si>
+    <t>0x000000060F060000</t>
+  </si>
+  <si>
+    <t>0x1B1B091200000000</t>
+  </si>
+  <si>
+    <t>0x09121B1B00000000</t>
+  </si>
+  <si>
+    <t>0x0102030300000000</t>
+  </si>
+  <si>
+    <t>0x0303010200000000</t>
   </si>
 </sst>
 </file>
@@ -5662,7 +6004,7 @@
         <v>224</v>
       </c>
       <c r="B194" t="str">
-        <f t="shared" ref="B194:B257" si="4">CHAR(A194)</f>
+        <f t="shared" ref="B194:B225" si="4">CHAR(A194)</f>
         <v>à</v>
       </c>
     </row>
@@ -5956,7 +6298,11 @@
   <dimension ref="A1:U227"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+      <pane xSplit="13830" ySplit="4755" topLeftCell="I103" activePane="bottomLeft"/>
+      <selection activeCell="D3" sqref="D3:D226"/>
+      <selection pane="topRight" activeCell="U10" sqref="U10"/>
+      <selection pane="bottomLeft" activeCell="C117" sqref="C117"/>
+      <selection pane="bottomRight" activeCell="Q116" sqref="Q116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6014,7 +6360,7 @@
     </row>
     <row r="2" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1">
@@ -6025,18 +6371,20 @@
       <c r="N2" s="13"/>
       <c r="O2" s="13"/>
       <c r="P2" s="13"/>
-      <c r="Q2" s="13">
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13">
         <v>1</v>
       </c>
-      <c r="R2" s="13"/>
-      <c r="S2" s="14"/>
+      <c r="S2" s="14">
+        <v>1</v>
+      </c>
       <c r="T2" s="10">
         <f t="array" ref="T2">SUMPRODUCT(L$1:S$1,IFERROR(LEN(L2:S2)/LEN(L2:S2),0))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U2" s="11">
         <f t="shared" ref="U2:U8" si="0">_xlfn.BITLSHIFT(T2,H$1*MOD(K2,4))</f>
-        <v>67108864</v>
+        <v>50331648</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
@@ -6044,10 +6392,10 @@
         <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E66" si="1">CHAR(A3)</f>
@@ -6063,21 +6411,21 @@
       <c r="M3" s="16"/>
       <c r="N3" s="16"/>
       <c r="O3" s="16"/>
-      <c r="P3" s="16">
-        <v>1</v>
-      </c>
+      <c r="P3" s="16"/>
       <c r="Q3" s="16"/>
       <c r="R3" s="16">
         <v>1</v>
       </c>
-      <c r="S3" s="17"/>
+      <c r="S3" s="17">
+        <v>1</v>
+      </c>
       <c r="T3" s="10">
         <f t="array" ref="T3">SUMPRODUCT(L$1:S$1,IFERROR(LEN(L3:S3)/LEN(L3:S3),0))</f>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="U3" s="11">
         <f t="shared" si="0"/>
-        <v>655360</v>
+        <v>196608</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
@@ -6085,17 +6433,17 @@
         <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="1"/>
         <v>!</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K4" s="1">
         <v>5</v>
@@ -6107,14 +6455,16 @@
       <c r="P4" s="16"/>
       <c r="Q4" s="16"/>
       <c r="R4" s="16"/>
-      <c r="S4" s="17"/>
+      <c r="S4" s="17">
+        <v>1</v>
+      </c>
       <c r="T4" s="10">
         <f t="array" ref="T4">SUMPRODUCT(L$1:S$1,IFERROR(LEN(L4:S4)/LEN(L4:S4),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U4" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
@@ -6122,10 +6472,10 @@
         <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="1"/>
@@ -6138,26 +6488,20 @@
       <c r="L5" s="15"/>
       <c r="M5" s="16"/>
       <c r="N5" s="16"/>
-      <c r="O5" s="16">
-        <v>1</v>
-      </c>
-      <c r="P5" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="16">
-        <v>1</v>
-      </c>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
       <c r="R5" s="16">
         <v>1</v>
       </c>
       <c r="S5" s="17"/>
       <c r="T5" s="10">
         <f t="array" ref="T5">SUMPRODUCT(L$1:S$1,IFERROR(LEN(L5:S5)/LEN(L5:S5),0))</f>
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="U5" s="11">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
@@ -6165,10 +6509,10 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="1"/>
@@ -6180,23 +6524,19 @@
       </c>
       <c r="L6" s="15"/>
       <c r="M6" s="16"/>
-      <c r="N6" s="16">
-        <v>1</v>
-      </c>
+      <c r="N6" s="16"/>
       <c r="O6" s="16"/>
       <c r="P6" s="16"/>
       <c r="Q6" s="16"/>
       <c r="R6" s="16"/>
-      <c r="S6" s="17">
-        <v>1</v>
-      </c>
+      <c r="S6" s="17"/>
       <c r="T6" s="10">
         <f t="array" ref="T6">SUMPRODUCT(L$1:S$1,IFERROR(LEN(L6:S6)/LEN(L6:S6),0))</f>
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="U6" s="11">
         <f t="shared" si="0"/>
-        <v>553648128</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
@@ -6204,10 +6544,10 @@
         <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="1"/>
@@ -6218,29 +6558,19 @@
       </c>
       <c r="L7" s="15"/>
       <c r="M7" s="16"/>
-      <c r="N7" s="16">
-        <v>1</v>
-      </c>
-      <c r="O7" s="16">
-        <v>1</v>
-      </c>
-      <c r="P7" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="16">
-        <v>1</v>
-      </c>
-      <c r="R7" s="16">
-        <v>1</v>
-      </c>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
       <c r="S7" s="17"/>
       <c r="T7" s="10">
         <f t="array" ref="T7">SUMPRODUCT(L$1:S$1,IFERROR(LEN(L7:S7)/LEN(L7:S7),0))</f>
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="U7" s="11">
         <f t="shared" si="0"/>
-        <v>4063232</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
@@ -6248,11 +6578,11 @@
         <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="1"/>
@@ -6264,9 +6594,7 @@
       </c>
       <c r="L8" s="15"/>
       <c r="M8" s="16"/>
-      <c r="N8" s="16">
-        <v>1</v>
-      </c>
+      <c r="N8" s="16"/>
       <c r="O8" s="16"/>
       <c r="P8" s="16"/>
       <c r="Q8" s="16"/>
@@ -6274,11 +6602,11 @@
       <c r="S8" s="17"/>
       <c r="T8" s="10">
         <f t="array" ref="T8">SUMPRODUCT(L$1:S$1,IFERROR(LEN(L8:S8)/LEN(L8:S8),0))</f>
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="U8" s="11">
         <f t="shared" si="0"/>
-        <v>8192</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
@@ -6286,10 +6614,10 @@
         <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="1"/>
@@ -6301,26 +6629,18 @@
       <c r="L9" s="18"/>
       <c r="M9" s="19"/>
       <c r="N9" s="19"/>
-      <c r="O9" s="19">
-        <v>1</v>
-      </c>
-      <c r="P9" s="19">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="19">
-        <v>1</v>
-      </c>
-      <c r="R9" s="19">
-        <v>1</v>
-      </c>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
       <c r="S9" s="20"/>
       <c r="T9" s="10">
         <f t="array" ref="T9">SUMPRODUCT(L$1:S$1,IFERROR(LEN(L9:S9)/LEN(L9:S9),0))</f>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="U9" s="11">
         <f>_xlfn.BITLSHIFT(T9,H$1*MOD(K9,4))</f>
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -6328,21 +6648,21 @@
         <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="1"/>
         <v>'</v>
       </c>
       <c r="L10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U10" s="8" t="str">
         <f>"0x"&amp;DEC2HEX(SUM(U2:U5),8)&amp;DEC2HEX(SUM(U6:U9),8)</f>
-        <v>0x040A001E213E201E</v>
+        <v>0x0303010200000000</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -6350,10 +6670,10 @@
         <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="1"/>
@@ -6365,10 +6685,10 @@
         <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="1"/>
@@ -6380,10 +6700,10 @@
         <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="1"/>
@@ -6395,10 +6715,10 @@
         <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="1"/>
@@ -6410,10 +6730,10 @@
         <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="1"/>
@@ -6425,10 +6745,10 @@
         <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="1"/>
@@ -6440,10 +6760,10 @@
         <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="1"/>
@@ -6455,10 +6775,10 @@
         <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="1"/>
@@ -6470,10 +6790,10 @@
         <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="1"/>
@@ -6485,10 +6805,10 @@
         <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="1"/>
@@ -6500,10 +6820,10 @@
         <v>50</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="1"/>
@@ -6515,10 +6835,10 @@
         <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="1"/>
@@ -6530,10 +6850,10 @@
         <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="1"/>
@@ -6545,10 +6865,10 @@
         <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="1"/>
@@ -6560,10 +6880,10 @@
         <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="1"/>
@@ -6575,10 +6895,10 @@
         <v>55</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="1"/>
@@ -6590,10 +6910,10 @@
         <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="1"/>
@@ -6605,10 +6925,10 @@
         <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="1"/>
@@ -6620,10 +6940,10 @@
         <v>58</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="1"/>
@@ -6635,10 +6955,10 @@
         <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="1"/>
@@ -6650,10 +6970,10 @@
         <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D31" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="1"/>
@@ -6665,10 +6985,10 @@
         <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="1"/>
@@ -6680,10 +7000,10 @@
         <v>62</v>
       </c>
       <c r="B33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="1"/>
@@ -6695,10 +7015,10 @@
         <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" si="1"/>
@@ -6710,10 +7030,10 @@
         <v>64</v>
       </c>
       <c r="B35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D35" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E35" t="str">
         <f t="shared" si="1"/>
@@ -6725,10 +7045,10 @@
         <v>65</v>
       </c>
       <c r="B36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D36" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E36" t="str">
         <f t="shared" si="1"/>
@@ -6740,10 +7060,10 @@
         <v>66</v>
       </c>
       <c r="B37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E37" t="str">
         <f t="shared" si="1"/>
@@ -6755,10 +7075,10 @@
         <v>67</v>
       </c>
       <c r="B38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D38" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E38" t="str">
         <f t="shared" si="1"/>
@@ -6770,10 +7090,10 @@
         <v>68</v>
       </c>
       <c r="B39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D39" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E39" t="str">
         <f t="shared" si="1"/>
@@ -6785,10 +7105,10 @@
         <v>69</v>
       </c>
       <c r="B40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D40" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" si="1"/>
@@ -6800,10 +7120,10 @@
         <v>70</v>
       </c>
       <c r="B41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D41" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E41" t="str">
         <f t="shared" si="1"/>
@@ -6815,10 +7135,10 @@
         <v>71</v>
       </c>
       <c r="B42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D42" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E42" t="str">
         <f t="shared" si="1"/>
@@ -6830,10 +7150,10 @@
         <v>72</v>
       </c>
       <c r="B43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D43" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E43" t="str">
         <f t="shared" si="1"/>
@@ -6845,10 +7165,10 @@
         <v>73</v>
       </c>
       <c r="B44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D44" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E44" t="str">
         <f t="shared" si="1"/>
@@ -6860,10 +7180,10 @@
         <v>74</v>
       </c>
       <c r="B45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D45" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E45" t="str">
         <f t="shared" si="1"/>
@@ -6875,10 +7195,10 @@
         <v>75</v>
       </c>
       <c r="B46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D46" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E46" t="str">
         <f t="shared" si="1"/>
@@ -6890,10 +7210,10 @@
         <v>76</v>
       </c>
       <c r="B47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D47" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E47" t="str">
         <f t="shared" si="1"/>
@@ -6905,10 +7225,10 @@
         <v>77</v>
       </c>
       <c r="B48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D48" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E48" t="str">
         <f t="shared" si="1"/>
@@ -6920,10 +7240,10 @@
         <v>78</v>
       </c>
       <c r="B49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D49" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E49" t="str">
         <f t="shared" si="1"/>
@@ -6935,10 +7255,10 @@
         <v>79</v>
       </c>
       <c r="B50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D50" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E50" t="str">
         <f t="shared" si="1"/>
@@ -6950,10 +7270,10 @@
         <v>80</v>
       </c>
       <c r="B51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D51" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E51" t="str">
         <f t="shared" si="1"/>
@@ -6965,10 +7285,10 @@
         <v>81</v>
       </c>
       <c r="B52" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D52" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E52" t="str">
         <f t="shared" si="1"/>
@@ -6980,10 +7300,10 @@
         <v>82</v>
       </c>
       <c r="B53" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D53" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E53" t="str">
         <f t="shared" si="1"/>
@@ -6995,10 +7315,10 @@
         <v>83</v>
       </c>
       <c r="B54" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D54" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E54" t="str">
         <f t="shared" si="1"/>
@@ -7010,10 +7330,10 @@
         <v>84</v>
       </c>
       <c r="B55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D55" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E55" t="str">
         <f t="shared" si="1"/>
@@ -7025,10 +7345,10 @@
         <v>85</v>
       </c>
       <c r="B56" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D56" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E56" t="str">
         <f t="shared" si="1"/>
@@ -7040,10 +7360,10 @@
         <v>86</v>
       </c>
       <c r="B57" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D57" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E57" t="str">
         <f t="shared" si="1"/>
@@ -7055,10 +7375,10 @@
         <v>87</v>
       </c>
       <c r="B58" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D58" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E58" t="str">
         <f t="shared" si="1"/>
@@ -7070,10 +7390,10 @@
         <v>88</v>
       </c>
       <c r="B59" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D59" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E59" t="str">
         <f t="shared" si="1"/>
@@ -7085,10 +7405,10 @@
         <v>89</v>
       </c>
       <c r="B60" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D60" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E60" t="str">
         <f t="shared" si="1"/>
@@ -7100,10 +7420,10 @@
         <v>90</v>
       </c>
       <c r="B61" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D61" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E61" t="str">
         <f t="shared" si="1"/>
@@ -7115,10 +7435,10 @@
         <v>91</v>
       </c>
       <c r="B62" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D62" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E62" t="str">
         <f t="shared" si="1"/>
@@ -7130,10 +7450,10 @@
         <v>92</v>
       </c>
       <c r="B63" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D63" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E63" t="str">
         <f t="shared" si="1"/>
@@ -7145,10 +7465,10 @@
         <v>93</v>
       </c>
       <c r="B64" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D64" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E64" t="str">
         <f t="shared" si="1"/>
@@ -7160,10 +7480,10 @@
         <v>94</v>
       </c>
       <c r="B65" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D65" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E65" t="str">
         <f t="shared" si="1"/>
@@ -7175,10 +7495,10 @@
         <v>95</v>
       </c>
       <c r="B66" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D66" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E66" t="str">
         <f t="shared" si="1"/>
@@ -7190,10 +7510,10 @@
         <v>96</v>
       </c>
       <c r="B67" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D67" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E67" t="str">
         <f t="shared" ref="E67:E130" si="2">CHAR(A67)</f>
@@ -7205,10 +7525,10 @@
         <v>97</v>
       </c>
       <c r="B68" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D68" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E68" t="str">
         <f t="shared" si="2"/>
@@ -7220,10 +7540,10 @@
         <v>98</v>
       </c>
       <c r="B69" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D69" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E69" t="str">
         <f t="shared" si="2"/>
@@ -7235,10 +7555,10 @@
         <v>99</v>
       </c>
       <c r="B70" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D70" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E70" t="str">
         <f t="shared" si="2"/>
@@ -7250,10 +7570,10 @@
         <v>100</v>
       </c>
       <c r="B71" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D71" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E71" t="str">
         <f t="shared" si="2"/>
@@ -7265,10 +7585,13 @@
         <v>101</v>
       </c>
       <c r="B72" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C72" t="s">
+        <v>16</v>
       </c>
       <c r="D72" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E72" t="str">
         <f t="shared" si="2"/>
@@ -7280,10 +7603,10 @@
         <v>102</v>
       </c>
       <c r="B73" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D73" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E73" t="str">
         <f t="shared" si="2"/>
@@ -7295,10 +7618,10 @@
         <v>103</v>
       </c>
       <c r="B74" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D74" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E74" t="str">
         <f t="shared" si="2"/>
@@ -7310,10 +7633,10 @@
         <v>104</v>
       </c>
       <c r="B75" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D75" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E75" t="str">
         <f t="shared" si="2"/>
@@ -7325,10 +7648,13 @@
         <v>105</v>
       </c>
       <c r="B76" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C76" t="s">
+        <v>25</v>
       </c>
       <c r="D76" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E76" t="str">
         <f t="shared" si="2"/>
@@ -7340,10 +7666,10 @@
         <v>106</v>
       </c>
       <c r="B77" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D77" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E77" t="str">
         <f t="shared" si="2"/>
@@ -7355,10 +7681,10 @@
         <v>107</v>
       </c>
       <c r="B78" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D78" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E78" t="str">
         <f t="shared" si="2"/>
@@ -7370,10 +7696,10 @@
         <v>108</v>
       </c>
       <c r="B79" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D79" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E79" t="str">
         <f t="shared" si="2"/>
@@ -7385,10 +7711,10 @@
         <v>109</v>
       </c>
       <c r="B80" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D80" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E80" t="str">
         <f t="shared" si="2"/>
@@ -7400,10 +7726,13 @@
         <v>110</v>
       </c>
       <c r="B81" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C81" t="s">
+        <v>27</v>
       </c>
       <c r="D81" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E81" t="str">
         <f t="shared" si="2"/>
@@ -7415,10 +7744,13 @@
         <v>111</v>
       </c>
       <c r="B82" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C82" t="s">
+        <v>34</v>
       </c>
       <c r="D82" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E82" t="str">
         <f t="shared" si="2"/>
@@ -7430,10 +7762,10 @@
         <v>112</v>
       </c>
       <c r="B83" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D83" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E83" t="str">
         <f t="shared" si="2"/>
@@ -7445,10 +7777,10 @@
         <v>113</v>
       </c>
       <c r="B84" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D84" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E84" t="str">
         <f t="shared" si="2"/>
@@ -7460,10 +7792,10 @@
         <v>114</v>
       </c>
       <c r="B85" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D85" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E85" t="str">
         <f t="shared" si="2"/>
@@ -7475,10 +7807,10 @@
         <v>115</v>
       </c>
       <c r="B86" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D86" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E86" t="str">
         <f t="shared" si="2"/>
@@ -7490,10 +7822,10 @@
         <v>116</v>
       </c>
       <c r="B87" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D87" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E87" t="str">
         <f t="shared" si="2"/>
@@ -7505,10 +7837,13 @@
         <v>117</v>
       </c>
       <c r="B88" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C88" t="s">
+        <v>41</v>
       </c>
       <c r="D88" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E88" t="str">
         <f t="shared" si="2"/>
@@ -7520,10 +7855,10 @@
         <v>118</v>
       </c>
       <c r="B89" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D89" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E89" t="str">
         <f t="shared" si="2"/>
@@ -7535,10 +7870,10 @@
         <v>119</v>
       </c>
       <c r="B90" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D90" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E90" t="str">
         <f t="shared" si="2"/>
@@ -7550,10 +7885,10 @@
         <v>120</v>
       </c>
       <c r="B91" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D91" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E91" t="str">
         <f t="shared" si="2"/>
@@ -7565,10 +7900,10 @@
         <v>121</v>
       </c>
       <c r="B92" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D92" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E92" t="str">
         <f t="shared" si="2"/>
@@ -7580,10 +7915,10 @@
         <v>122</v>
       </c>
       <c r="B93" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D93" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E93" t="str">
         <f t="shared" si="2"/>
@@ -7595,10 +7930,10 @@
         <v>123</v>
       </c>
       <c r="B94" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D94" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E94" t="str">
         <f t="shared" si="2"/>
@@ -7610,10 +7945,10 @@
         <v>124</v>
       </c>
       <c r="B95" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D95" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E95" t="str">
         <f t="shared" si="2"/>
@@ -7625,10 +7960,10 @@
         <v>125</v>
       </c>
       <c r="B96" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D96" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E96" t="str">
         <f t="shared" si="2"/>
@@ -7640,10 +7975,10 @@
         <v>126</v>
       </c>
       <c r="B97" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D97" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E97" t="str">
         <f t="shared" si="2"/>
@@ -7655,10 +7990,10 @@
         <v>127</v>
       </c>
       <c r="B98" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D98" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E98" t="str">
         <f t="shared" si="2"/>
@@ -7670,10 +8005,10 @@
         <v>128</v>
       </c>
       <c r="B99" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D99" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E99" t="str">
         <f t="shared" si="2"/>
@@ -7685,10 +8020,10 @@
         <v>129</v>
       </c>
       <c r="B100" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D100" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E100" t="str">
         <f t="shared" si="2"/>
@@ -7700,10 +8035,10 @@
         <v>130</v>
       </c>
       <c r="B101" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D101" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E101" t="str">
         <f t="shared" si="2"/>
@@ -7715,10 +8050,10 @@
         <v>131</v>
       </c>
       <c r="B102" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D102" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E102" t="str">
         <f t="shared" si="2"/>
@@ -7730,10 +8065,10 @@
         <v>132</v>
       </c>
       <c r="B103" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D103" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E103" t="str">
         <f t="shared" si="2"/>
@@ -7745,10 +8080,10 @@
         <v>133</v>
       </c>
       <c r="B104" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D104" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E104" t="str">
         <f t="shared" si="2"/>
@@ -7760,10 +8095,10 @@
         <v>134</v>
       </c>
       <c r="B105" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D105" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E105" t="str">
         <f t="shared" si="2"/>
@@ -7775,10 +8110,10 @@
         <v>135</v>
       </c>
       <c r="B106" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D106" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E106" t="str">
         <f t="shared" si="2"/>
@@ -7790,10 +8125,10 @@
         <v>136</v>
       </c>
       <c r="B107" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D107" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E107" t="str">
         <f t="shared" si="2"/>
@@ -7805,10 +8140,10 @@
         <v>137</v>
       </c>
       <c r="B108" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D108" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E108" t="str">
         <f t="shared" si="2"/>
@@ -7820,10 +8155,10 @@
         <v>138</v>
       </c>
       <c r="B109" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D109" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E109" t="str">
         <f t="shared" si="2"/>
@@ -7835,10 +8170,10 @@
         <v>139</v>
       </c>
       <c r="B110" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D110" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E110" t="str">
         <f t="shared" si="2"/>
@@ -7850,10 +8185,13 @@
         <v>140</v>
       </c>
       <c r="B111" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C111" t="s">
+        <v>119</v>
       </c>
       <c r="D111" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E111" t="str">
         <f t="shared" si="2"/>
@@ -7865,10 +8203,10 @@
         <v>141</v>
       </c>
       <c r="B112" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D112" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E112" t="str">
         <f t="shared" si="2"/>
@@ -7880,10 +8218,10 @@
         <v>142</v>
       </c>
       <c r="B113" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D113" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E113" t="str">
         <f t="shared" si="2"/>
@@ -7895,10 +8233,10 @@
         <v>143</v>
       </c>
       <c r="B114" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D114" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E114" t="str">
         <f t="shared" si="2"/>
@@ -7910,10 +8248,10 @@
         <v>144</v>
       </c>
       <c r="B115" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D115" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E115" t="str">
         <f t="shared" si="2"/>
@@ -7925,10 +8263,13 @@
         <v>145</v>
       </c>
       <c r="B116" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C116" t="s">
+        <v>129</v>
       </c>
       <c r="D116" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E116" t="str">
         <f t="shared" si="2"/>
@@ -7940,10 +8281,13 @@
         <v>146</v>
       </c>
       <c r="B117" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C117" t="s">
+        <v>130</v>
       </c>
       <c r="D117" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E117" t="str">
         <f t="shared" si="2"/>
@@ -7955,10 +8299,13 @@
         <v>147</v>
       </c>
       <c r="B118" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C118" t="s">
+        <v>128</v>
       </c>
       <c r="D118" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E118" t="str">
         <f t="shared" si="2"/>
@@ -7970,10 +8317,13 @@
         <v>148</v>
       </c>
       <c r="B119" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C119" t="s">
+        <v>127</v>
       </c>
       <c r="D119" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E119" t="str">
         <f t="shared" si="2"/>
@@ -7985,10 +8335,13 @@
         <v>149</v>
       </c>
       <c r="B120" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C120" t="s">
+        <v>126</v>
       </c>
       <c r="D120" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E120" t="str">
         <f t="shared" si="2"/>
@@ -8000,10 +8353,13 @@
         <v>150</v>
       </c>
       <c r="B121" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C121" t="s">
+        <v>125</v>
       </c>
       <c r="D121" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E121" t="str">
         <f t="shared" si="2"/>
@@ -8015,10 +8371,13 @@
         <v>151</v>
       </c>
       <c r="B122" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C122" t="s">
+        <v>124</v>
       </c>
       <c r="D122" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E122" t="str">
         <f t="shared" si="2"/>
@@ -8030,10 +8389,13 @@
         <v>152</v>
       </c>
       <c r="B123" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C123" t="s">
+        <v>123</v>
       </c>
       <c r="D123" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E123" t="str">
         <f t="shared" si="2"/>
@@ -8045,10 +8407,13 @@
         <v>153</v>
       </c>
       <c r="B124" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C124" t="s">
+        <v>122</v>
       </c>
       <c r="D124" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E124" t="str">
         <f t="shared" si="2"/>
@@ -8060,10 +8425,13 @@
         <v>154</v>
       </c>
       <c r="B125" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C125" t="s">
+        <v>121</v>
       </c>
       <c r="D125" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E125" t="str">
         <f t="shared" si="2"/>
@@ -8075,10 +8443,13 @@
         <v>155</v>
       </c>
       <c r="B126" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C126" t="s">
+        <v>120</v>
       </c>
       <c r="D126" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E126" t="str">
         <f t="shared" si="2"/>
@@ -8090,10 +8461,13 @@
         <v>156</v>
       </c>
       <c r="B127" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C127" t="s">
+        <v>118</v>
       </c>
       <c r="D127" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E127" t="str">
         <f t="shared" si="2"/>
@@ -8105,10 +8479,10 @@
         <v>157</v>
       </c>
       <c r="B128" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D128" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E128" t="str">
         <f t="shared" si="2"/>
@@ -8120,10 +8494,13 @@
         <v>158</v>
       </c>
       <c r="B129" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C129" t="s">
+        <v>117</v>
       </c>
       <c r="D129" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E129" t="str">
         <f t="shared" si="2"/>
@@ -8135,10 +8512,13 @@
         <v>159</v>
       </c>
       <c r="B130" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C130" t="s">
+        <v>116</v>
       </c>
       <c r="D130" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E130" t="str">
         <f t="shared" si="2"/>
@@ -8150,10 +8530,10 @@
         <v>160</v>
       </c>
       <c r="B131" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D131" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E131" t="str">
         <f t="shared" ref="E131:E194" si="3">CHAR(A131)</f>
@@ -8165,10 +8545,13 @@
         <v>161</v>
       </c>
       <c r="B132" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C132" t="s">
+        <v>115</v>
       </c>
       <c r="D132" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E132" t="str">
         <f t="shared" si="3"/>
@@ -8180,10 +8563,13 @@
         <v>162</v>
       </c>
       <c r="B133" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C133" t="s">
+        <v>114</v>
       </c>
       <c r="D133" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E133" t="str">
         <f t="shared" si="3"/>
@@ -8195,10 +8581,13 @@
         <v>163</v>
       </c>
       <c r="B134" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C134" t="s">
+        <v>113</v>
       </c>
       <c r="D134" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E134" t="str">
         <f t="shared" si="3"/>
@@ -8210,10 +8599,13 @@
         <v>164</v>
       </c>
       <c r="B135" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C135" t="s">
+        <v>112</v>
       </c>
       <c r="D135" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E135" t="str">
         <f t="shared" si="3"/>
@@ -8225,10 +8617,13 @@
         <v>165</v>
       </c>
       <c r="B136" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C136" t="s">
+        <v>111</v>
       </c>
       <c r="D136" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E136" t="str">
         <f t="shared" si="3"/>
@@ -8240,10 +8635,13 @@
         <v>166</v>
       </c>
       <c r="B137" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C137" t="s">
+        <v>110</v>
       </c>
       <c r="D137" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E137" t="str">
         <f t="shared" si="3"/>
@@ -8255,10 +8653,13 @@
         <v>167</v>
       </c>
       <c r="B138" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C138" t="s">
+        <v>109</v>
       </c>
       <c r="D138" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E138" t="str">
         <f t="shared" si="3"/>
@@ -8270,10 +8671,13 @@
         <v>168</v>
       </c>
       <c r="B139" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C139" t="s">
+        <v>108</v>
       </c>
       <c r="D139" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E139" t="str">
         <f t="shared" si="3"/>
@@ -8285,10 +8689,13 @@
         <v>169</v>
       </c>
       <c r="B140" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C140" t="s">
+        <v>107</v>
       </c>
       <c r="D140" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E140" t="str">
         <f t="shared" si="3"/>
@@ -8300,10 +8707,13 @@
         <v>170</v>
       </c>
       <c r="B141" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C141" t="s">
+        <v>106</v>
       </c>
       <c r="D141" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E141" t="str">
         <f t="shared" si="3"/>
@@ -8315,10 +8725,13 @@
         <v>171</v>
       </c>
       <c r="B142" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C142" t="s">
+        <v>105</v>
       </c>
       <c r="D142" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E142" t="str">
         <f t="shared" si="3"/>
@@ -8330,10 +8743,13 @@
         <v>172</v>
       </c>
       <c r="B143" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C143" t="s">
+        <v>104</v>
       </c>
       <c r="D143" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E143" t="str">
         <f t="shared" si="3"/>
@@ -8345,10 +8761,13 @@
         <v>173</v>
       </c>
       <c r="B144" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C144" t="s">
+        <v>103</v>
       </c>
       <c r="D144" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E144" t="str">
         <f t="shared" si="3"/>
@@ -8360,10 +8779,13 @@
         <v>174</v>
       </c>
       <c r="B145" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C145" t="s">
+        <v>102</v>
       </c>
       <c r="D145" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E145" t="str">
         <f t="shared" si="3"/>
@@ -8375,10 +8797,13 @@
         <v>175</v>
       </c>
       <c r="B146" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C146" t="s">
+        <v>101</v>
       </c>
       <c r="D146" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E146" t="str">
         <f t="shared" si="3"/>
@@ -8390,10 +8815,13 @@
         <v>176</v>
       </c>
       <c r="B147" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C147" t="s">
+        <v>100</v>
       </c>
       <c r="D147" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E147" t="str">
         <f t="shared" si="3"/>
@@ -8405,10 +8833,13 @@
         <v>177</v>
       </c>
       <c r="B148" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C148" t="s">
+        <v>99</v>
       </c>
       <c r="D148" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E148" t="str">
         <f t="shared" si="3"/>
@@ -8420,10 +8851,13 @@
         <v>178</v>
       </c>
       <c r="B149" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C149" t="s">
+        <v>98</v>
       </c>
       <c r="D149" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E149" t="str">
         <f t="shared" si="3"/>
@@ -8435,10 +8869,13 @@
         <v>179</v>
       </c>
       <c r="B150" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C150" t="s">
+        <v>97</v>
       </c>
       <c r="D150" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E150" t="str">
         <f t="shared" si="3"/>
@@ -8450,10 +8887,13 @@
         <v>180</v>
       </c>
       <c r="B151" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C151" t="s">
+        <v>96</v>
       </c>
       <c r="D151" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E151" t="str">
         <f t="shared" si="3"/>
@@ -8465,10 +8905,13 @@
         <v>181</v>
       </c>
       <c r="B152" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C152" t="s">
+        <v>95</v>
       </c>
       <c r="D152" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E152" t="str">
         <f t="shared" si="3"/>
@@ -8480,10 +8923,13 @@
         <v>182</v>
       </c>
       <c r="B153" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C153" t="s">
+        <v>94</v>
       </c>
       <c r="D153" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E153" t="str">
         <f t="shared" si="3"/>
@@ -8495,10 +8941,13 @@
         <v>183</v>
       </c>
       <c r="B154" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C154" t="s">
+        <v>93</v>
       </c>
       <c r="D154" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E154" t="str">
         <f t="shared" si="3"/>
@@ -8510,10 +8959,13 @@
         <v>184</v>
       </c>
       <c r="B155" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C155" t="s">
+        <v>92</v>
       </c>
       <c r="D155" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E155" t="str">
         <f t="shared" si="3"/>
@@ -8525,10 +8977,13 @@
         <v>185</v>
       </c>
       <c r="B156" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C156" t="s">
+        <v>91</v>
       </c>
       <c r="D156" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E156" t="str">
         <f t="shared" si="3"/>
@@ -8540,10 +8995,13 @@
         <v>186</v>
       </c>
       <c r="B157" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C157" t="s">
+        <v>90</v>
       </c>
       <c r="D157" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E157" t="str">
         <f t="shared" si="3"/>
@@ -8555,10 +9013,13 @@
         <v>187</v>
       </c>
       <c r="B158" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C158" t="s">
+        <v>89</v>
       </c>
       <c r="D158" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E158" t="str">
         <f t="shared" si="3"/>
@@ -8570,10 +9031,13 @@
         <v>188</v>
       </c>
       <c r="B159" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C159" t="s">
+        <v>86</v>
       </c>
       <c r="D159" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E159" t="str">
         <f t="shared" si="3"/>
@@ -8585,10 +9049,13 @@
         <v>189</v>
       </c>
       <c r="B160" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C160" t="s">
+        <v>87</v>
       </c>
       <c r="D160" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E160" t="str">
         <f t="shared" si="3"/>
@@ -8600,10 +9067,13 @@
         <v>190</v>
       </c>
       <c r="B161" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C161" t="s">
+        <v>88</v>
       </c>
       <c r="D161" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E161" t="str">
         <f t="shared" si="3"/>
@@ -8615,10 +9085,13 @@
         <v>191</v>
       </c>
       <c r="B162" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C162" t="s">
+        <v>85</v>
       </c>
       <c r="D162" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E162" t="str">
         <f t="shared" si="3"/>
@@ -8630,10 +9103,13 @@
         <v>192</v>
       </c>
       <c r="B163" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C163" t="s">
+        <v>84</v>
       </c>
       <c r="D163" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E163" t="str">
         <f t="shared" si="3"/>
@@ -8645,10 +9121,13 @@
         <v>193</v>
       </c>
       <c r="B164" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C164" t="s">
+        <v>83</v>
       </c>
       <c r="D164" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E164" t="str">
         <f t="shared" si="3"/>
@@ -8660,10 +9139,13 @@
         <v>194</v>
       </c>
       <c r="B165" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C165" t="s">
+        <v>82</v>
       </c>
       <c r="D165" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E165" t="str">
         <f t="shared" si="3"/>
@@ -8675,10 +9157,13 @@
         <v>195</v>
       </c>
       <c r="B166" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C166" t="s">
+        <v>81</v>
       </c>
       <c r="D166" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E166" t="str">
         <f t="shared" si="3"/>
@@ -8690,10 +9175,13 @@
         <v>196</v>
       </c>
       <c r="B167" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C167" t="s">
+        <v>80</v>
       </c>
       <c r="D167" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E167" t="str">
         <f t="shared" si="3"/>
@@ -8705,10 +9193,13 @@
         <v>197</v>
       </c>
       <c r="B168" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C168" t="s">
+        <v>79</v>
       </c>
       <c r="D168" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E168" t="str">
         <f t="shared" si="3"/>
@@ -8720,10 +9211,13 @@
         <v>198</v>
       </c>
       <c r="B169" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C169" t="s">
+        <v>78</v>
       </c>
       <c r="D169" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E169" t="str">
         <f t="shared" si="3"/>
@@ -8735,10 +9229,13 @@
         <v>199</v>
       </c>
       <c r="B170" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C170" t="s">
+        <v>77</v>
       </c>
       <c r="D170" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E170" t="str">
         <f t="shared" si="3"/>
@@ -8750,10 +9247,13 @@
         <v>200</v>
       </c>
       <c r="B171" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C171" t="s">
+        <v>76</v>
       </c>
       <c r="D171" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E171" t="str">
         <f t="shared" si="3"/>
@@ -8765,10 +9265,13 @@
         <v>201</v>
       </c>
       <c r="B172" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C172" t="s">
+        <v>75</v>
       </c>
       <c r="D172" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E172" t="str">
         <f t="shared" si="3"/>
@@ -8780,10 +9283,13 @@
         <v>202</v>
       </c>
       <c r="B173" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C173" t="s">
+        <v>74</v>
       </c>
       <c r="D173" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E173" t="str">
         <f t="shared" si="3"/>
@@ -8795,10 +9301,13 @@
         <v>203</v>
       </c>
       <c r="B174" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C174" t="s">
+        <v>73</v>
       </c>
       <c r="D174" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E174" t="str">
         <f t="shared" si="3"/>
@@ -8810,10 +9319,13 @@
         <v>204</v>
       </c>
       <c r="B175" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C175" t="s">
+        <v>72</v>
       </c>
       <c r="D175" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E175" t="str">
         <f t="shared" si="3"/>
@@ -8825,10 +9337,13 @@
         <v>205</v>
       </c>
       <c r="B176" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C176" t="s">
+        <v>71</v>
       </c>
       <c r="D176" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E176" t="str">
         <f t="shared" si="3"/>
@@ -8840,10 +9355,13 @@
         <v>206</v>
       </c>
       <c r="B177" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C177" t="s">
+        <v>70</v>
       </c>
       <c r="D177" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E177" t="str">
         <f t="shared" si="3"/>
@@ -8855,10 +9373,13 @@
         <v>207</v>
       </c>
       <c r="B178" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C178" t="s">
+        <v>69</v>
       </c>
       <c r="D178" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E178" t="str">
         <f t="shared" si="3"/>
@@ -8870,10 +9391,13 @@
         <v>208</v>
       </c>
       <c r="B179" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C179" t="s">
+        <v>68</v>
       </c>
       <c r="D179" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E179" t="str">
         <f t="shared" si="3"/>
@@ -8885,10 +9409,13 @@
         <v>209</v>
       </c>
       <c r="B180" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C180" t="s">
+        <v>67</v>
       </c>
       <c r="D180" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E180" t="str">
         <f t="shared" si="3"/>
@@ -8900,10 +9427,13 @@
         <v>210</v>
       </c>
       <c r="B181" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C181" t="s">
+        <v>64</v>
       </c>
       <c r="D181" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E181" t="str">
         <f t="shared" si="3"/>
@@ -8915,10 +9445,13 @@
         <v>211</v>
       </c>
       <c r="B182" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C182" t="s">
+        <v>63</v>
       </c>
       <c r="D182" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E182" t="str">
         <f t="shared" si="3"/>
@@ -8930,10 +9463,13 @@
         <v>212</v>
       </c>
       <c r="B183" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C183" t="s">
+        <v>62</v>
       </c>
       <c r="D183" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E183" t="str">
         <f t="shared" si="3"/>
@@ -8945,10 +9481,13 @@
         <v>213</v>
       </c>
       <c r="B184" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C184" t="s">
+        <v>61</v>
       </c>
       <c r="D184" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E184" t="str">
         <f t="shared" si="3"/>
@@ -8960,10 +9499,13 @@
         <v>214</v>
       </c>
       <c r="B185" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C185" t="s">
+        <v>60</v>
       </c>
       <c r="D185" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E185" t="str">
         <f t="shared" si="3"/>
@@ -8975,10 +9517,13 @@
         <v>215</v>
       </c>
       <c r="B186" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C186" t="s">
+        <v>65</v>
       </c>
       <c r="D186" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E186" t="str">
         <f t="shared" si="3"/>
@@ -8990,10 +9535,13 @@
         <v>216</v>
       </c>
       <c r="B187" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C187" t="s">
+        <v>66</v>
       </c>
       <c r="D187" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E187" t="str">
         <f t="shared" si="3"/>
@@ -9005,10 +9553,13 @@
         <v>217</v>
       </c>
       <c r="B188" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C188" t="s">
+        <v>59</v>
       </c>
       <c r="D188" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E188" t="str">
         <f t="shared" si="3"/>
@@ -9020,10 +9571,13 @@
         <v>218</v>
       </c>
       <c r="B189" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C189" t="s">
+        <v>58</v>
       </c>
       <c r="D189" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E189" t="str">
         <f t="shared" si="3"/>
@@ -9035,10 +9589,13 @@
         <v>219</v>
       </c>
       <c r="B190" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C190" t="s">
+        <v>56</v>
       </c>
       <c r="D190" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E190" t="str">
         <f t="shared" si="3"/>
@@ -9050,10 +9607,13 @@
         <v>220</v>
       </c>
       <c r="B191" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C191" t="s">
+        <v>57</v>
       </c>
       <c r="D191" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E191" t="str">
         <f t="shared" si="3"/>
@@ -9065,10 +9625,13 @@
         <v>221</v>
       </c>
       <c r="B192" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C192" t="s">
+        <v>55</v>
       </c>
       <c r="D192" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E192" t="str">
         <f t="shared" si="3"/>
@@ -9080,10 +9643,13 @@
         <v>222</v>
       </c>
       <c r="B193" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C193" t="s">
+        <v>53</v>
       </c>
       <c r="D193" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E193" t="str">
         <f t="shared" si="3"/>
@@ -9095,10 +9661,13 @@
         <v>223</v>
       </c>
       <c r="B194" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C194" t="s">
+        <v>54</v>
       </c>
       <c r="D194" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E194" t="str">
         <f t="shared" si="3"/>
@@ -9110,13 +9679,16 @@
         <v>224</v>
       </c>
       <c r="B195" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C195" t="s">
+        <v>51</v>
       </c>
       <c r="D195" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E195" t="str">
-        <f>CHAR(A195)</f>
+        <f t="shared" ref="E195:E226" si="4">CHAR(A195)</f>
         <v>à</v>
       </c>
     </row>
@@ -9125,13 +9697,16 @@
         <v>225</v>
       </c>
       <c r="B196" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C196" t="s">
+        <v>52</v>
       </c>
       <c r="D196" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E196" t="str">
-        <f>CHAR(A196)</f>
+        <f t="shared" si="4"/>
         <v>á</v>
       </c>
     </row>
@@ -9140,13 +9715,16 @@
         <v>226</v>
       </c>
       <c r="B197" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C197" t="s">
+        <v>50</v>
       </c>
       <c r="D197" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E197" t="str">
-        <f>CHAR(A197)</f>
+        <f t="shared" si="4"/>
         <v>â</v>
       </c>
     </row>
@@ -9155,13 +9733,16 @@
         <v>227</v>
       </c>
       <c r="B198" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C198" t="s">
+        <v>49</v>
       </c>
       <c r="D198" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E198" t="str">
-        <f>CHAR(A198)</f>
+        <f t="shared" si="4"/>
         <v>ã</v>
       </c>
     </row>
@@ -9170,13 +9751,16 @@
         <v>228</v>
       </c>
       <c r="B199" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C199" t="s">
+        <v>48</v>
       </c>
       <c r="D199" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E199" t="str">
-        <f>CHAR(A199)</f>
+        <f t="shared" si="4"/>
         <v>ä</v>
       </c>
     </row>
@@ -9185,13 +9769,16 @@
         <v>229</v>
       </c>
       <c r="B200" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C200" t="s">
+        <v>47</v>
       </c>
       <c r="D200" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E200" t="str">
-        <f>CHAR(A200)</f>
+        <f t="shared" si="4"/>
         <v>å</v>
       </c>
     </row>
@@ -9200,13 +9787,16 @@
         <v>230</v>
       </c>
       <c r="B201" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C201" t="s">
+        <v>46</v>
       </c>
       <c r="D201" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E201" t="str">
-        <f>CHAR(A201)</f>
+        <f t="shared" si="4"/>
         <v>æ</v>
       </c>
     </row>
@@ -9215,13 +9805,16 @@
         <v>231</v>
       </c>
       <c r="B202" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C202" t="s">
+        <v>45</v>
       </c>
       <c r="D202" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E202" t="str">
-        <f>CHAR(A202)</f>
+        <f t="shared" si="4"/>
         <v>ç</v>
       </c>
     </row>
@@ -9230,13 +9823,16 @@
         <v>232</v>
       </c>
       <c r="B203" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C203" t="s">
+        <v>18</v>
       </c>
       <c r="D203" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E203" t="str">
-        <f>CHAR(A203)</f>
+        <f t="shared" si="4"/>
         <v>è</v>
       </c>
     </row>
@@ -9245,13 +9841,16 @@
         <v>233</v>
       </c>
       <c r="B204" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C204" t="s">
+        <v>17</v>
       </c>
       <c r="D204" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E204" t="str">
-        <f>CHAR(A204)</f>
+        <f t="shared" si="4"/>
         <v>é</v>
       </c>
     </row>
@@ -9260,16 +9859,16 @@
         <v>234</v>
       </c>
       <c r="B205" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C205" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D205" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E205" t="str">
-        <f>CHAR(A205)</f>
+        <f t="shared" si="4"/>
         <v>ê</v>
       </c>
     </row>
@@ -9278,13 +9877,16 @@
         <v>235</v>
       </c>
       <c r="B206" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C206" t="s">
+        <v>19</v>
       </c>
       <c r="D206" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E206" t="str">
-        <f>CHAR(A206)</f>
+        <f t="shared" si="4"/>
         <v>ë</v>
       </c>
     </row>
@@ -9293,13 +9895,16 @@
         <v>236</v>
       </c>
       <c r="B207" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C207" t="s">
+        <v>23</v>
       </c>
       <c r="D207" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E207" t="str">
-        <f>CHAR(A207)</f>
+        <f t="shared" si="4"/>
         <v>ì</v>
       </c>
     </row>
@@ -9308,13 +9913,16 @@
         <v>237</v>
       </c>
       <c r="B208" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C208" t="s">
+        <v>24</v>
       </c>
       <c r="D208" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E208" t="str">
-        <f>CHAR(A208)</f>
+        <f t="shared" si="4"/>
         <v>í</v>
       </c>
     </row>
@@ -9323,13 +9931,16 @@
         <v>238</v>
       </c>
       <c r="B209" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C209" t="s">
+        <v>21</v>
       </c>
       <c r="D209" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E209" t="str">
-        <f>CHAR(A209)</f>
+        <f t="shared" si="4"/>
         <v>î</v>
       </c>
     </row>
@@ -9338,13 +9949,16 @@
         <v>239</v>
       </c>
       <c r="B210" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C210" t="s">
+        <v>20</v>
       </c>
       <c r="D210" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E210" t="str">
-        <f>CHAR(A210)</f>
+        <f t="shared" si="4"/>
         <v>ï</v>
       </c>
     </row>
@@ -9353,13 +9967,16 @@
         <v>240</v>
       </c>
       <c r="B211" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C211" t="s">
+        <v>28</v>
       </c>
       <c r="D211" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E211" t="str">
-        <f>CHAR(A211)</f>
+        <f t="shared" si="4"/>
         <v>ð</v>
       </c>
     </row>
@@ -9368,13 +9985,16 @@
         <v>241</v>
       </c>
       <c r="B212" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C212" t="s">
+        <v>26</v>
       </c>
       <c r="D212" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E212" t="str">
-        <f>CHAR(A212)</f>
+        <f t="shared" si="4"/>
         <v>ñ</v>
       </c>
     </row>
@@ -9383,13 +10003,16 @@
         <v>242</v>
       </c>
       <c r="B213" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C213" t="s">
+        <v>29</v>
       </c>
       <c r="D213" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E213" t="str">
-        <f>CHAR(A213)</f>
+        <f t="shared" si="4"/>
         <v>ò</v>
       </c>
     </row>
@@ -9398,13 +10021,16 @@
         <v>243</v>
       </c>
       <c r="B214" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C214" t="s">
+        <v>30</v>
       </c>
       <c r="D214" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E214" t="str">
-        <f>CHAR(A214)</f>
+        <f t="shared" si="4"/>
         <v>ó</v>
       </c>
     </row>
@@ -9413,13 +10039,16 @@
         <v>244</v>
       </c>
       <c r="B215" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C215" t="s">
+        <v>31</v>
       </c>
       <c r="D215" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E215" t="str">
-        <f>CHAR(A215)</f>
+        <f t="shared" si="4"/>
         <v>ô</v>
       </c>
     </row>
@@ -9428,13 +10057,16 @@
         <v>245</v>
       </c>
       <c r="B216" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C216" t="s">
+        <v>32</v>
       </c>
       <c r="D216" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E216" t="str">
-        <f>CHAR(A216)</f>
+        <f t="shared" si="4"/>
         <v>õ</v>
       </c>
     </row>
@@ -9443,13 +10075,16 @@
         <v>246</v>
       </c>
       <c r="B217" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C217" t="s">
+        <v>33</v>
       </c>
       <c r="D217" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E217" t="str">
-        <f>CHAR(A217)</f>
+        <f t="shared" si="4"/>
         <v>ö</v>
       </c>
     </row>
@@ -9458,13 +10093,16 @@
         <v>247</v>
       </c>
       <c r="B218" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C218" t="s">
+        <v>35</v>
       </c>
       <c r="D218" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E218" t="str">
-        <f>CHAR(A218)</f>
+        <f t="shared" si="4"/>
         <v>÷</v>
       </c>
     </row>
@@ -9473,13 +10111,16 @@
         <v>248</v>
       </c>
       <c r="B219" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C219" t="s">
+        <v>36</v>
       </c>
       <c r="D219" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E219" t="str">
-        <f>CHAR(A219)</f>
+        <f t="shared" si="4"/>
         <v>ø</v>
       </c>
     </row>
@@ -9488,13 +10129,16 @@
         <v>249</v>
       </c>
       <c r="B220" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C220" t="s">
+        <v>37</v>
       </c>
       <c r="D220" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E220" t="str">
-        <f>CHAR(A220)</f>
+        <f t="shared" si="4"/>
         <v>ù</v>
       </c>
     </row>
@@ -9503,13 +10147,16 @@
         <v>250</v>
       </c>
       <c r="B221" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C221" t="s">
+        <v>38</v>
       </c>
       <c r="D221" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E221" t="str">
-        <f>CHAR(A221)</f>
+        <f t="shared" si="4"/>
         <v>ú</v>
       </c>
     </row>
@@ -9518,13 +10165,16 @@
         <v>251</v>
       </c>
       <c r="B222" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C222" t="s">
+        <v>39</v>
       </c>
       <c r="D222" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E222" t="str">
-        <f>CHAR(A222)</f>
+        <f t="shared" si="4"/>
         <v>û</v>
       </c>
     </row>
@@ -9533,13 +10183,16 @@
         <v>252</v>
       </c>
       <c r="B223" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C223" t="s">
+        <v>40</v>
       </c>
       <c r="D223" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E223" t="str">
-        <f>CHAR(A223)</f>
+        <f t="shared" si="4"/>
         <v>ü</v>
       </c>
     </row>
@@ -9548,13 +10201,16 @@
         <v>253</v>
       </c>
       <c r="B224" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C224" t="s">
+        <v>42</v>
       </c>
       <c r="D224" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E224" t="str">
-        <f>CHAR(A224)</f>
+        <f t="shared" si="4"/>
         <v>ý</v>
       </c>
     </row>
@@ -9563,13 +10219,16 @@
         <v>254</v>
       </c>
       <c r="B225" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C225" t="s">
+        <v>43</v>
       </c>
       <c r="D225" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E225" t="str">
-        <f>CHAR(A225)</f>
+        <f t="shared" si="4"/>
         <v>þ</v>
       </c>
     </row>
@@ -9578,19 +10237,22 @@
         <v>255</v>
       </c>
       <c r="B226" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C226" t="s">
+        <v>44</v>
       </c>
       <c r="D226" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E226" t="str">
-        <f>CHAR(A226)</f>
+        <f t="shared" si="4"/>
         <v>ÿ</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 8x8 font and tests
</commit_message>
<xml_diff>
--- a/BigAsciiChars.xlsx
+++ b/BigAsciiChars.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD675179-7F2A-4540-81A3-9EFE64230C68}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD9B2F3-C331-4C83-9AF7-6B2121BA347B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1695" yWindow="60" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{6D1A8F03-DA32-4E55-9CE4-87A60CFBC80E}"/>
+    <workbookView xWindow="2835" yWindow="2625" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{6D1A8F03-DA32-4E55-9CE4-87A60CFBC80E}"/>
   </bookViews>
   <sheets>
     <sheet name="5x5" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="236">
   <si>
     <t>Code</t>
   </si>
@@ -105,9 +105,6 @@
     <t>0x0102000202020202</t>
   </si>
   <si>
-    <t>0x0000020002020202</t>
-  </si>
-  <si>
     <t>0x0A14002C32222222</t>
   </si>
   <si>
@@ -141,21 +138,6 @@
     <t>0x00011E2529313E40</t>
   </si>
   <si>
-    <t>0x000804111111110E</t>
-  </si>
-  <si>
-    <t>0x000204111111110E</t>
-  </si>
-  <si>
-    <t>0x040A00111111110E</t>
-  </si>
-  <si>
-    <t>0x000A00111111110E</t>
-  </si>
-  <si>
-    <t>0x000000111111110E</t>
-  </si>
-  <si>
     <t>0x000204110A040810</t>
   </si>
   <si>
@@ -421,13 +403,346 @@
   </si>
   <si>
     <t>0x0303010200000000</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>0xFC8284FC828182FC</t>
+  </si>
+  <si>
+    <t>0x7E8180808080817E</t>
+  </si>
+  <si>
+    <t>0xFC828181818182FC</t>
+  </si>
+  <si>
+    <t>0x3C428181FF818181</t>
+  </si>
+  <si>
+    <t>0xFE8080F8808080FF</t>
+  </si>
+  <si>
+    <t>0x7F40407C40404040</t>
+  </si>
+  <si>
+    <t>0x1F2040BCC281413E</t>
+  </si>
+  <si>
+    <t>0x3F4080809E81413F</t>
+  </si>
+  <si>
+    <t>0x4141417F41414141</t>
+  </si>
+  <si>
+    <t>0x0702020202020207</t>
+  </si>
+  <si>
+    <t>0x1F0202020242423E</t>
+  </si>
+  <si>
+    <t>0x2126283028242221</t>
+  </si>
+  <si>
+    <t>0x404040404040407F</t>
+  </si>
+  <si>
+    <t>0x6699999999998181</t>
+  </si>
+  <si>
+    <t>0x4163554949414141</t>
+  </si>
+  <si>
+    <t>0xC1E1B1998D878381</t>
+  </si>
+  <si>
+    <t>0x81C1A19189858381</t>
+  </si>
+  <si>
+    <t>0x3C4281818181423C</t>
+  </si>
+  <si>
+    <t>0x7E4141417E404040</t>
+  </si>
+  <si>
+    <t>0x3E41414141493E01</t>
+  </si>
+  <si>
+    <t>0xFC828284F8848281</t>
+  </si>
+  <si>
+    <t>0x3C4242700C42423C</t>
+  </si>
+  <si>
+    <t>0x7F08080808080808</t>
+  </si>
+  <si>
+    <t>0x4141414141221408</t>
+  </si>
+  <si>
+    <t>0x8181424224241818</t>
+  </si>
+  <si>
+    <t>0x414141414141413E</t>
+  </si>
+  <si>
+    <t>0x414949494949493E</t>
+  </si>
+  <si>
+    <t>0x818181425A5A2424</t>
+  </si>
+  <si>
+    <t>0x8142241818244281</t>
+  </si>
+  <si>
+    <t>0x8142241810204080</t>
+  </si>
+  <si>
+    <t>0xFF020408102040FF</t>
+  </si>
+  <si>
+    <t>0x0704040404040407</t>
+  </si>
+  <si>
+    <t>0x1008080404020201</t>
+  </si>
+  <si>
+    <t>0x0102020404080810</t>
+  </si>
+  <si>
+    <t>0x0701010101010107</t>
+  </si>
+  <si>
+    <t>0x040A110000000000</t>
+  </si>
+  <si>
+    <t>0x000000000000007F</t>
+  </si>
+  <si>
+    <t>0x0403000000000000</t>
+  </si>
+  <si>
+    <t>0x1E21210204080008</t>
+  </si>
+  <si>
+    <t>0x7C82BDA5BF80413E</t>
+  </si>
+  <si>
+    <t>0xC0300C03030C30C0</t>
+  </si>
+  <si>
+    <t>0x030C30C0C0300C03</t>
+  </si>
+  <si>
+    <t>0x0000007F007F0000</t>
+  </si>
+  <si>
+    <t>0x0000010000000100</t>
+  </si>
+  <si>
+    <t>0x0000010000010200</t>
+  </si>
+  <si>
+    <t>0x1E2121211F020C30</t>
+  </si>
+  <si>
+    <t>0x3E4141413E41413E</t>
+  </si>
+  <si>
+    <t>0x7E01020408102040</t>
+  </si>
+  <si>
+    <t>0x7F40403C0201413E</t>
+  </si>
+  <si>
+    <t>0x404040447F040404</t>
+  </si>
+  <si>
+    <t>0x1E2101011E01413E</t>
+  </si>
+  <si>
+    <t>0x3E4141061820403F</t>
+  </si>
+  <si>
+    <t>0x0206020202020207</t>
+  </si>
+  <si>
+    <t>0x1C2241414141221C</t>
+  </si>
+  <si>
+    <t>0x0402010101010204</t>
+  </si>
+  <si>
+    <t>0x0102040404040201</t>
+  </si>
+  <si>
+    <t>0x0049493E083E4949</t>
+  </si>
+  <si>
+    <t>0x000008087F080800</t>
+  </si>
+  <si>
+    <t>0x0000000000000102</t>
+  </si>
+  <si>
+    <t>0x0000000000000303</t>
+  </si>
+  <si>
+    <t>0x0001010000000000</t>
+  </si>
+  <si>
+    <t>0x384444283D45423D</t>
+  </si>
+  <si>
+    <t>0x0071527408172547</t>
+  </si>
+  <si>
+    <t>0x083E48483E093E08</t>
+  </si>
+  <si>
+    <t>0x12127F12127F1212</t>
+  </si>
+  <si>
+    <t>0x0505000000000000</t>
+  </si>
+  <si>
+    <t>0x0101010101010001</t>
+  </si>
+  <si>
+    <t>0x00001E01011F111F</t>
+  </si>
+  <si>
+    <t>0x00001E212020211E</t>
+  </si>
+  <si>
+    <t>0x000101010F11110F</t>
+  </si>
+  <si>
+    <t>0x002020203E21213E</t>
+  </si>
+  <si>
+    <t>0x00000E091C080808</t>
+  </si>
+  <si>
+    <t>0x00000F111F01211E</t>
+  </si>
+  <si>
+    <t>0x0020202C32212121</t>
+  </si>
+  <si>
+    <t>0x0002000202020201</t>
+  </si>
+  <si>
+    <t>0x0001000101010906</t>
+  </si>
+  <si>
+    <t>0x00080B0C080C0A09</t>
+  </si>
+  <si>
+    <t>0x0002020202020201</t>
+  </si>
+  <si>
+    <t>0x0000323D29292121</t>
+  </si>
+  <si>
+    <t>0x00001719111E1010</t>
+  </si>
+  <si>
+    <t>0x00000D13110F0101</t>
+  </si>
+  <si>
+    <t>0x0000171810101010</t>
+  </si>
+  <si>
+    <t>0x00000E100E01010E</t>
+  </si>
+  <si>
+    <t>0x00101C101010111E</t>
+  </si>
+  <si>
+    <t>0x000021212121231D</t>
+  </si>
+  <si>
+    <t>0x140021212121231D</t>
+  </si>
+  <si>
+    <t>0x040821212121231D</t>
+  </si>
+  <si>
+    <t>0x080421212121231D</t>
+  </si>
+  <si>
+    <t>0x040A21212121231D</t>
+  </si>
+  <si>
+    <t>0x000021212121120C</t>
+  </si>
+  <si>
+    <t>0x0000414141492A14</t>
+  </si>
+  <si>
+    <t>0x000011110A0C0A11</t>
+  </si>
+  <si>
+    <t>0x000021211E022418</t>
+  </si>
+  <si>
+    <t>0x00003E030408103F</t>
+  </si>
+  <si>
+    <t>0x0306040202040403</t>
+  </si>
+  <si>
+    <t>0x0603010202010106</t>
+  </si>
+  <si>
+    <t>0x0101010101010101</t>
+  </si>
+  <si>
+    <t>0x3F2121212121213F</t>
+  </si>
+  <si>
+    <t>0x3E41407C4078413E</t>
+  </si>
+  <si>
+    <t>0x0302070202020206</t>
+  </si>
+  <si>
+    <t>0x000000000000050A</t>
+  </si>
+  <si>
+    <t>0x0000000000000015</t>
+  </si>
+  <si>
+    <t>0x0002070202020200</t>
+  </si>
+  <si>
+    <t>0x0002070202070200</t>
+  </si>
+  <si>
+    <t>0x0002050000000000</t>
+  </si>
+  <si>
+    <t>0x00C2C40810205B9B</t>
+  </si>
+  <si>
+    <t>0xA040E11100E011E</t>
+  </si>
+  <si>
+    <t>0x0000000102040201</t>
+  </si>
+  <si>
+    <t>0x0A043F020408103F</t>
+  </si>
+  <si>
+    <t>space</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -468,6 +783,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Amboy Black"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -570,7 +892,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -587,15 +909,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6297,12 +6622,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F29B42-D457-474D-80E0-5F35A50E03D1}">
   <dimension ref="A1:U227"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="13830" ySplit="4755" topLeftCell="I103" activePane="bottomLeft"/>
-      <selection activeCell="D3" sqref="D3:D226"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="10605" ySplit="3780" activePane="bottomLeft"/>
+      <selection activeCell="R75" sqref="R75"/>
       <selection pane="topRight" activeCell="U10" sqref="U10"/>
-      <selection pane="bottomLeft" activeCell="C117" sqref="C117"/>
-      <selection pane="bottomRight" activeCell="Q116" sqref="Q116"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="U87" sqref="U87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6358,7 +6683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:21" ht="18" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -6366,40 +6691,42 @@
       <c r="K2" s="1">
         <v>7</v>
       </c>
-      <c r="L2" s="12"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13">
-        <v>1</v>
-      </c>
-      <c r="S2" s="14">
-        <v>1</v>
-      </c>
+      <c r="L2" s="13"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="S2" s="15"/>
       <c r="T2" s="10">
         <f t="array" ref="T2">SUMPRODUCT(L$1:S$1,IFERROR(LEN(L2:S2)/LEN(L2:S2),0))</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="U2" s="11">
         <f t="shared" ref="U2:U8" si="0">_xlfn.BITLSHIFT(T2,H$1*MOD(K2,4))</f>
-        <v>50331648</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
+        <v>167772160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="18" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>32</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
       <c r="D3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" t="str">
-        <f t="shared" ref="E3:E66" si="1">CHAR(A3)</f>
-        <v xml:space="preserve"> </v>
+      <c r="E3" t="s">
+        <v>235</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>5</v>
@@ -6407,39 +6734,40 @@
       <c r="K3" s="1">
         <v>6</v>
       </c>
-      <c r="L3" s="15"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16">
-        <v>1</v>
-      </c>
-      <c r="S3" s="17">
-        <v>1</v>
-      </c>
+      <c r="L3" s="16"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="R3" s="18"/>
+      <c r="S3" s="19"/>
       <c r="T3" s="10">
         <f t="array" ref="T3">SUMPRODUCT(L$1:S$1,IFERROR(LEN(L3:S3)/LEN(L3:S3),0))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U3" s="11">
         <f t="shared" si="0"/>
-        <v>196608</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="18" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>33</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
+      <c r="C4" t="s">
+        <v>192</v>
+      </c>
       <c r="D4" t="s">
         <v>22</v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="E3:E66" si="1">CHAR(A4)</f>
         <v>!</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -6448,31 +6776,44 @@
       <c r="K4" s="1">
         <v>5</v>
       </c>
-      <c r="L4" s="15"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="17">
-        <v>1</v>
+      <c r="L4" s="16"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="P4" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q4" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="R4" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="S4" s="19" t="s">
+        <v>125</v>
       </c>
       <c r="T4" s="10">
         <f t="array" ref="T4">SUMPRODUCT(L$1:S$1,IFERROR(LEN(L4:S4)/LEN(L4:S4),0))</f>
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="U4" s="11">
         <f t="shared" si="0"/>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
+        <v>16128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="18" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>34</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>191</v>
       </c>
       <c r="D5" t="s">
         <v>22</v>
@@ -6485,16 +6826,16 @@
       <c r="K5" s="1">
         <v>4</v>
       </c>
-      <c r="L5" s="15"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16">
-        <v>1</v>
-      </c>
-      <c r="S5" s="17"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="S5" s="20"/>
       <c r="T5" s="10">
         <f t="array" ref="T5">SUMPRODUCT(L$1:S$1,IFERROR(LEN(L5:S5)/LEN(L5:S5),0))</f>
         <v>2</v>
@@ -6504,12 +6845,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:21" ht="18" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>35</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>190</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
@@ -6522,29 +6866,34 @@
       <c r="K6" s="1">
         <v>3</v>
       </c>
-      <c r="L6" s="15"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="17"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="R6" s="17"/>
+      <c r="S6" s="20"/>
       <c r="T6" s="10">
         <f t="array" ref="T6">SUMPRODUCT(L$1:S$1,IFERROR(LEN(L6:S6)/LEN(L6:S6),0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U6" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
+        <v>67108864</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="18" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>36</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>189</v>
       </c>
       <c r="D7" t="s">
         <v>22</v>
@@ -6556,31 +6905,35 @@
       <c r="K7" s="1">
         <v>2</v>
       </c>
-      <c r="L7" s="15"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="17"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="20"/>
       <c r="T7" s="10">
         <f t="array" ref="T7">SUMPRODUCT(L$1:S$1,IFERROR(LEN(L7:S7)/LEN(L7:S7),0))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U7" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
+        <v>524288</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="18" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>37</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="12" t="s">
+        <v>188</v>
+      </c>
       <c r="D8" t="s">
         <v>22</v>
       </c>
@@ -6592,29 +6945,34 @@
       <c r="K8" s="1">
         <v>1</v>
       </c>
-      <c r="L8" s="15"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="17"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="20"/>
       <c r="T8" s="10">
         <f t="array" ref="T8">SUMPRODUCT(L$1:S$1,IFERROR(LEN(L8:S8)/LEN(L8:S8),0))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="U8" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="18" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>38</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>187</v>
       </c>
       <c r="D9" t="s">
         <v>22</v>
@@ -6626,21 +6984,33 @@
       <c r="K9" s="1">
         <v>0</v>
       </c>
-      <c r="L9" s="18"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="20"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="O9" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="P9" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q9" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="R9" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="S9" s="23" t="s">
+        <v>125</v>
+      </c>
       <c r="T9" s="10">
         <f t="array" ref="T9">SUMPRODUCT(L$1:S$1,IFERROR(LEN(L9:S9)/LEN(L9:S9),0))</f>
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="U9" s="11">
         <f>_xlfn.BITLSHIFT(T9,H$1*MOD(K9,4))</f>
-        <v>0</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -6650,6 +7020,9 @@
       <c r="B10" t="s">
         <v>10</v>
       </c>
+      <c r="C10" t="s">
+        <v>186</v>
+      </c>
       <c r="D10" t="s">
         <v>22</v>
       </c>
@@ -6662,7 +7035,7 @@
       </c>
       <c r="U10" s="8" t="str">
         <f>"0x"&amp;DEC2HEX(SUM(U2:U5),8)&amp;DEC2HEX(SUM(U6:U9),8)</f>
-        <v>0x0303010200000000</v>
+        <v>0x0A043F020408103F</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -6672,6 +7045,9 @@
       <c r="B11" t="s">
         <v>10</v>
       </c>
+      <c r="C11" t="s">
+        <v>181</v>
+      </c>
       <c r="D11" t="s">
         <v>22</v>
       </c>
@@ -6687,6 +7063,9 @@
       <c r="B12" t="s">
         <v>10</v>
       </c>
+      <c r="C12" t="s">
+        <v>180</v>
+      </c>
       <c r="D12" t="s">
         <v>22</v>
       </c>
@@ -6702,6 +7081,9 @@
       <c r="B13" t="s">
         <v>10</v>
       </c>
+      <c r="C13" t="s">
+        <v>182</v>
+      </c>
       <c r="D13" t="s">
         <v>22</v>
       </c>
@@ -6717,6 +7099,9 @@
       <c r="B14" t="s">
         <v>10</v>
       </c>
+      <c r="C14" t="s">
+        <v>183</v>
+      </c>
       <c r="D14" t="s">
         <v>22</v>
       </c>
@@ -6732,6 +7117,9 @@
       <c r="B15" t="s">
         <v>10</v>
       </c>
+      <c r="C15" t="s">
+        <v>184</v>
+      </c>
       <c r="D15" t="s">
         <v>22</v>
       </c>
@@ -6747,6 +7135,9 @@
       <c r="B16" t="s">
         <v>10</v>
       </c>
+      <c r="C16" t="s">
+        <v>119</v>
+      </c>
       <c r="D16" t="s">
         <v>22</v>
       </c>
@@ -6762,6 +7153,9 @@
       <c r="B17" t="s">
         <v>10</v>
       </c>
+      <c r="C17" t="s">
+        <v>185</v>
+      </c>
       <c r="D17" t="s">
         <v>22</v>
       </c>
@@ -6777,6 +7171,9 @@
       <c r="B18" t="s">
         <v>10</v>
       </c>
+      <c r="C18" t="s">
+        <v>159</v>
+      </c>
       <c r="D18" t="s">
         <v>22</v>
       </c>
@@ -6792,6 +7189,9 @@
       <c r="B19" t="s">
         <v>10</v>
       </c>
+      <c r="C19" t="s">
+        <v>179</v>
+      </c>
       <c r="D19" t="s">
         <v>22</v>
       </c>
@@ -6807,6 +7207,9 @@
       <c r="B20" t="s">
         <v>10</v>
       </c>
+      <c r="C20" t="s">
+        <v>178</v>
+      </c>
       <c r="D20" t="s">
         <v>22</v>
       </c>
@@ -6822,6 +7225,9 @@
       <c r="B21" t="s">
         <v>10</v>
       </c>
+      <c r="C21" t="s">
+        <v>177</v>
+      </c>
       <c r="D21" t="s">
         <v>22</v>
       </c>
@@ -6837,6 +7243,9 @@
       <c r="B22" t="s">
         <v>10</v>
       </c>
+      <c r="C22" t="s">
+        <v>176</v>
+      </c>
       <c r="D22" t="s">
         <v>22</v>
       </c>
@@ -6852,6 +7261,9 @@
       <c r="B23" t="s">
         <v>10</v>
       </c>
+      <c r="C23" t="s">
+        <v>175</v>
+      </c>
       <c r="D23" t="s">
         <v>22</v>
       </c>
@@ -6867,6 +7279,9 @@
       <c r="B24" t="s">
         <v>10</v>
       </c>
+      <c r="C24" t="s">
+        <v>174</v>
+      </c>
       <c r="D24" t="s">
         <v>22</v>
       </c>
@@ -6882,6 +7297,9 @@
       <c r="B25" t="s">
         <v>10</v>
       </c>
+      <c r="C25" t="s">
+        <v>132</v>
+      </c>
       <c r="D25" t="s">
         <v>22</v>
       </c>
@@ -6897,6 +7315,9 @@
       <c r="B26" t="s">
         <v>10</v>
       </c>
+      <c r="C26" t="s">
+        <v>173</v>
+      </c>
       <c r="D26" t="s">
         <v>22</v>
       </c>
@@ -6912,6 +7333,9 @@
       <c r="B27" t="s">
         <v>10</v>
       </c>
+      <c r="C27" t="s">
+        <v>172</v>
+      </c>
       <c r="D27" t="s">
         <v>22</v>
       </c>
@@ -6927,6 +7351,9 @@
       <c r="B28" t="s">
         <v>10</v>
       </c>
+      <c r="C28" t="s">
+        <v>171</v>
+      </c>
       <c r="D28" t="s">
         <v>22</v>
       </c>
@@ -6942,6 +7369,9 @@
       <c r="B29" t="s">
         <v>10</v>
       </c>
+      <c r="C29" t="s">
+        <v>169</v>
+      </c>
       <c r="D29" t="s">
         <v>22</v>
       </c>
@@ -6957,6 +7387,9 @@
       <c r="B30" t="s">
         <v>10</v>
       </c>
+      <c r="C30" t="s">
+        <v>170</v>
+      </c>
       <c r="D30" t="s">
         <v>22</v>
       </c>
@@ -6972,6 +7405,9 @@
       <c r="B31" t="s">
         <v>10</v>
       </c>
+      <c r="C31" t="s">
+        <v>167</v>
+      </c>
       <c r="D31" t="s">
         <v>22</v>
       </c>
@@ -6987,6 +7423,9 @@
       <c r="B32" t="s">
         <v>10</v>
       </c>
+      <c r="C32" t="s">
+        <v>168</v>
+      </c>
       <c r="D32" t="s">
         <v>22</v>
       </c>
@@ -6995,12 +7434,15 @@
         <v>=</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>62</v>
       </c>
       <c r="B33" t="s">
         <v>10</v>
+      </c>
+      <c r="C33" t="s">
+        <v>166</v>
       </c>
       <c r="D33" t="s">
         <v>22</v>
@@ -7010,12 +7452,15 @@
         <v>&gt;</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>63</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
+      </c>
+      <c r="C34" t="s">
+        <v>164</v>
       </c>
       <c r="D34" t="s">
         <v>22</v>
@@ -7025,12 +7470,15 @@
         <v>?</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>64</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
+      </c>
+      <c r="C35" t="s">
+        <v>165</v>
       </c>
       <c r="D35" t="s">
         <v>22</v>
@@ -7040,12 +7488,15 @@
         <v>@</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>65</v>
       </c>
       <c r="B36" t="s">
         <v>10</v>
+      </c>
+      <c r="C36" t="s">
+        <v>129</v>
       </c>
       <c r="D36" t="s">
         <v>22</v>
@@ -7055,12 +7506,15 @@
         <v>A</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>66</v>
       </c>
       <c r="B37" t="s">
         <v>10</v>
+      </c>
+      <c r="C37" t="s">
+        <v>126</v>
       </c>
       <c r="D37" t="s">
         <v>22</v>
@@ -7070,12 +7524,15 @@
         <v>B</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>67</v>
       </c>
       <c r="B38" t="s">
         <v>10</v>
+      </c>
+      <c r="C38" t="s">
+        <v>127</v>
       </c>
       <c r="D38" t="s">
         <v>22</v>
@@ -7085,12 +7542,15 @@
         <v>C</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>68</v>
       </c>
       <c r="B39" t="s">
         <v>10</v>
+      </c>
+      <c r="C39" t="s">
+        <v>128</v>
       </c>
       <c r="D39" t="s">
         <v>22</v>
@@ -7100,12 +7560,15 @@
         <v>D</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>69</v>
       </c>
       <c r="B40" t="s">
         <v>10</v>
+      </c>
+      <c r="C40" t="s">
+        <v>130</v>
       </c>
       <c r="D40" t="s">
         <v>22</v>
@@ -7115,12 +7578,15 @@
         <v>E</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>70</v>
       </c>
       <c r="B41" t="s">
         <v>10</v>
+      </c>
+      <c r="C41" t="s">
+        <v>131</v>
       </c>
       <c r="D41" t="s">
         <v>22</v>
@@ -7130,12 +7596,15 @@
         <v>F</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>71</v>
       </c>
       <c r="B42" t="s">
         <v>10</v>
+      </c>
+      <c r="C42" t="s">
+        <v>133</v>
       </c>
       <c r="D42" t="s">
         <v>22</v>
@@ -7145,12 +7614,15 @@
         <v>G</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>72</v>
       </c>
       <c r="B43" t="s">
         <v>10</v>
+      </c>
+      <c r="C43" t="s">
+        <v>134</v>
       </c>
       <c r="D43" t="s">
         <v>22</v>
@@ -7160,12 +7632,15 @@
         <v>H</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>73</v>
       </c>
       <c r="B44" t="s">
         <v>10</v>
+      </c>
+      <c r="C44" t="s">
+        <v>135</v>
       </c>
       <c r="D44" t="s">
         <v>22</v>
@@ -7175,12 +7650,15 @@
         <v>I</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>74</v>
       </c>
       <c r="B45" t="s">
         <v>10</v>
+      </c>
+      <c r="C45" t="s">
+        <v>136</v>
       </c>
       <c r="D45" t="s">
         <v>22</v>
@@ -7190,12 +7668,15 @@
         <v>J</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>75</v>
       </c>
       <c r="B46" t="s">
         <v>10</v>
+      </c>
+      <c r="C46" t="s">
+        <v>137</v>
       </c>
       <c r="D46" t="s">
         <v>22</v>
@@ -7205,12 +7686,15 @@
         <v>K</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>76</v>
       </c>
       <c r="B47" t="s">
         <v>10</v>
+      </c>
+      <c r="C47" t="s">
+        <v>138</v>
       </c>
       <c r="D47" t="s">
         <v>22</v>
@@ -7220,12 +7704,15 @@
         <v>L</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>77</v>
       </c>
       <c r="B48" t="s">
         <v>10</v>
+      </c>
+      <c r="C48" t="s">
+        <v>140</v>
       </c>
       <c r="D48" t="s">
         <v>22</v>
@@ -7234,13 +7721,19 @@
         <f t="shared" si="1"/>
         <v>M</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>78</v>
       </c>
       <c r="B49" t="s">
         <v>10</v>
+      </c>
+      <c r="C49" t="s">
+        <v>142</v>
       </c>
       <c r="D49" t="s">
         <v>22</v>
@@ -7249,13 +7742,19 @@
         <f t="shared" si="1"/>
         <v>N</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>79</v>
       </c>
       <c r="B50" t="s">
         <v>10</v>
+      </c>
+      <c r="C50" t="s">
+        <v>143</v>
       </c>
       <c r="D50" t="s">
         <v>22</v>
@@ -7265,12 +7764,15 @@
         <v>O</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>80</v>
       </c>
       <c r="B51" t="s">
         <v>10</v>
+      </c>
+      <c r="C51" t="s">
+        <v>144</v>
       </c>
       <c r="D51" t="s">
         <v>22</v>
@@ -7280,12 +7782,15 @@
         <v>P</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>81</v>
       </c>
       <c r="B52" t="s">
         <v>10</v>
+      </c>
+      <c r="C52" t="s">
+        <v>145</v>
       </c>
       <c r="D52" t="s">
         <v>22</v>
@@ -7295,12 +7800,15 @@
         <v>Q</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>82</v>
       </c>
       <c r="B53" t="s">
         <v>10</v>
+      </c>
+      <c r="C53" t="s">
+        <v>146</v>
       </c>
       <c r="D53" t="s">
         <v>22</v>
@@ -7310,12 +7818,15 @@
         <v>R</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>83</v>
       </c>
       <c r="B54" t="s">
         <v>10</v>
+      </c>
+      <c r="C54" t="s">
+        <v>147</v>
       </c>
       <c r="D54" t="s">
         <v>22</v>
@@ -7325,12 +7836,15 @@
         <v>S</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>84</v>
       </c>
       <c r="B55" t="s">
         <v>10</v>
+      </c>
+      <c r="C55" t="s">
+        <v>148</v>
       </c>
       <c r="D55" t="s">
         <v>22</v>
@@ -7340,12 +7854,15 @@
         <v>T</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>85</v>
       </c>
       <c r="B56" t="s">
         <v>10</v>
+      </c>
+      <c r="C56" t="s">
+        <v>151</v>
       </c>
       <c r="D56" t="s">
         <v>22</v>
@@ -7355,12 +7872,15 @@
         <v>U</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>86</v>
       </c>
       <c r="B57" t="s">
         <v>10</v>
+      </c>
+      <c r="C57" t="s">
+        <v>150</v>
       </c>
       <c r="D57" t="s">
         <v>22</v>
@@ -7369,13 +7889,19 @@
         <f t="shared" si="1"/>
         <v>V</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>87</v>
       </c>
       <c r="B58" t="s">
         <v>10</v>
+      </c>
+      <c r="C58" t="s">
+        <v>153</v>
       </c>
       <c r="D58" t="s">
         <v>22</v>
@@ -7384,13 +7910,19 @@
         <f t="shared" si="1"/>
         <v>W</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>88</v>
       </c>
       <c r="B59" t="s">
         <v>10</v>
+      </c>
+      <c r="C59" t="s">
+        <v>154</v>
       </c>
       <c r="D59" t="s">
         <v>22</v>
@@ -7400,12 +7932,15 @@
         <v>X</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>89</v>
       </c>
       <c r="B60" t="s">
         <v>10</v>
+      </c>
+      <c r="C60" t="s">
+        <v>155</v>
       </c>
       <c r="D60" t="s">
         <v>22</v>
@@ -7415,12 +7950,15 @@
         <v>Y</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>90</v>
       </c>
       <c r="B61" t="s">
         <v>10</v>
+      </c>
+      <c r="C61" t="s">
+        <v>156</v>
       </c>
       <c r="D61" t="s">
         <v>22</v>
@@ -7430,12 +7968,15 @@
         <v>Z</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>91</v>
       </c>
       <c r="B62" t="s">
         <v>10</v>
+      </c>
+      <c r="C62" t="s">
+        <v>157</v>
       </c>
       <c r="D62" t="s">
         <v>22</v>
@@ -7445,12 +7986,15 @@
         <v>[</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>92</v>
       </c>
       <c r="B63" t="s">
         <v>10</v>
+      </c>
+      <c r="C63" t="s">
+        <v>158</v>
       </c>
       <c r="D63" t="s">
         <v>22</v>
@@ -7460,12 +8004,15 @@
         <v>\</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>93</v>
       </c>
       <c r="B64" t="s">
         <v>10</v>
+      </c>
+      <c r="C64" t="s">
+        <v>160</v>
       </c>
       <c r="D64" t="s">
         <v>22</v>
@@ -7482,6 +8029,9 @@
       <c r="B65" t="s">
         <v>10</v>
       </c>
+      <c r="C65" t="s">
+        <v>161</v>
+      </c>
       <c r="D65" t="s">
         <v>22</v>
       </c>
@@ -7497,6 +8047,9 @@
       <c r="B66" t="s">
         <v>10</v>
       </c>
+      <c r="C66" t="s">
+        <v>162</v>
+      </c>
       <c r="D66" t="s">
         <v>22</v>
       </c>
@@ -7512,6 +8065,9 @@
       <c r="B67" t="s">
         <v>10</v>
       </c>
+      <c r="C67" t="s">
+        <v>163</v>
+      </c>
       <c r="D67" t="s">
         <v>22</v>
       </c>
@@ -7527,6 +8083,9 @@
       <c r="B68" t="s">
         <v>10</v>
       </c>
+      <c r="C68" t="s">
+        <v>193</v>
+      </c>
       <c r="D68" t="s">
         <v>22</v>
       </c>
@@ -7542,6 +8101,9 @@
       <c r="B69" t="s">
         <v>10</v>
       </c>
+      <c r="C69" t="s">
+        <v>196</v>
+      </c>
       <c r="D69" t="s">
         <v>22</v>
       </c>
@@ -7557,6 +8119,9 @@
       <c r="B70" t="s">
         <v>10</v>
       </c>
+      <c r="C70" t="s">
+        <v>194</v>
+      </c>
       <c r="D70" t="s">
         <v>22</v>
       </c>
@@ -7572,6 +8137,9 @@
       <c r="B71" t="s">
         <v>10</v>
       </c>
+      <c r="C71" t="s">
+        <v>195</v>
+      </c>
       <c r="D71" t="s">
         <v>22</v>
       </c>
@@ -7605,6 +8173,9 @@
       <c r="B73" t="s">
         <v>10</v>
       </c>
+      <c r="C73" t="s">
+        <v>197</v>
+      </c>
       <c r="D73" t="s">
         <v>22</v>
       </c>
@@ -7620,6 +8191,9 @@
       <c r="B74" t="s">
         <v>10</v>
       </c>
+      <c r="C74" t="s">
+        <v>198</v>
+      </c>
       <c r="D74" t="s">
         <v>22</v>
       </c>
@@ -7635,6 +8209,9 @@
       <c r="B75" t="s">
         <v>10</v>
       </c>
+      <c r="C75" t="s">
+        <v>199</v>
+      </c>
       <c r="D75" t="s">
         <v>22</v>
       </c>
@@ -7651,7 +8228,7 @@
         <v>10</v>
       </c>
       <c r="C76" t="s">
-        <v>25</v>
+        <v>200</v>
       </c>
       <c r="D76" t="s">
         <v>22</v>
@@ -7668,6 +8245,9 @@
       <c r="B77" t="s">
         <v>10</v>
       </c>
+      <c r="C77" t="s">
+        <v>201</v>
+      </c>
       <c r="D77" t="s">
         <v>22</v>
       </c>
@@ -7683,6 +8263,9 @@
       <c r="B78" t="s">
         <v>10</v>
       </c>
+      <c r="C78" t="s">
+        <v>202</v>
+      </c>
       <c r="D78" t="s">
         <v>22</v>
       </c>
@@ -7698,6 +8281,9 @@
       <c r="B79" t="s">
         <v>10</v>
       </c>
+      <c r="C79" t="s">
+        <v>203</v>
+      </c>
       <c r="D79" t="s">
         <v>22</v>
       </c>
@@ -7713,6 +8299,9 @@
       <c r="B80" t="s">
         <v>10</v>
       </c>
+      <c r="C80" t="s">
+        <v>204</v>
+      </c>
       <c r="D80" t="s">
         <v>22</v>
       </c>
@@ -7729,7 +8318,7 @@
         <v>10</v>
       </c>
       <c r="C81" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D81" t="s">
         <v>22</v>
@@ -7747,7 +8336,7 @@
         <v>10</v>
       </c>
       <c r="C82" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D82" t="s">
         <v>22</v>
@@ -7764,6 +8353,9 @@
       <c r="B83" t="s">
         <v>10</v>
       </c>
+      <c r="C83" t="s">
+        <v>205</v>
+      </c>
       <c r="D83" t="s">
         <v>22</v>
       </c>
@@ -7779,6 +8371,9 @@
       <c r="B84" t="s">
         <v>10</v>
       </c>
+      <c r="C84" t="s">
+        <v>206</v>
+      </c>
       <c r="D84" t="s">
         <v>22</v>
       </c>
@@ -7794,6 +8389,9 @@
       <c r="B85" t="s">
         <v>10</v>
       </c>
+      <c r="C85" t="s">
+        <v>207</v>
+      </c>
       <c r="D85" t="s">
         <v>22</v>
       </c>
@@ -7809,6 +8407,9 @@
       <c r="B86" t="s">
         <v>10</v>
       </c>
+      <c r="C86" t="s">
+        <v>208</v>
+      </c>
       <c r="D86" t="s">
         <v>22</v>
       </c>
@@ -7824,6 +8425,9 @@
       <c r="B87" t="s">
         <v>10</v>
       </c>
+      <c r="C87" t="s">
+        <v>209</v>
+      </c>
       <c r="D87" t="s">
         <v>22</v>
       </c>
@@ -7840,7 +8444,7 @@
         <v>10</v>
       </c>
       <c r="C88" t="s">
-        <v>41</v>
+        <v>210</v>
       </c>
       <c r="D88" t="s">
         <v>22</v>
@@ -7857,6 +8461,9 @@
       <c r="B89" t="s">
         <v>10</v>
       </c>
+      <c r="C89" t="s">
+        <v>215</v>
+      </c>
       <c r="D89" t="s">
         <v>22</v>
       </c>
@@ -7872,6 +8479,9 @@
       <c r="B90" t="s">
         <v>10</v>
       </c>
+      <c r="C90" t="s">
+        <v>216</v>
+      </c>
       <c r="D90" t="s">
         <v>22</v>
       </c>
@@ -7887,6 +8497,9 @@
       <c r="B91" t="s">
         <v>10</v>
       </c>
+      <c r="C91" t="s">
+        <v>217</v>
+      </c>
       <c r="D91" t="s">
         <v>22</v>
       </c>
@@ -7902,6 +8515,9 @@
       <c r="B92" t="s">
         <v>10</v>
       </c>
+      <c r="C92" t="s">
+        <v>218</v>
+      </c>
       <c r="D92" t="s">
         <v>22</v>
       </c>
@@ -7917,6 +8533,9 @@
       <c r="B93" t="s">
         <v>10</v>
       </c>
+      <c r="C93" t="s">
+        <v>219</v>
+      </c>
       <c r="D93" t="s">
         <v>22</v>
       </c>
@@ -7932,6 +8551,9 @@
       <c r="B94" t="s">
         <v>10</v>
       </c>
+      <c r="C94" t="s">
+        <v>220</v>
+      </c>
       <c r="D94" t="s">
         <v>22</v>
       </c>
@@ -7947,6 +8569,9 @@
       <c r="B95" t="s">
         <v>10</v>
       </c>
+      <c r="C95" t="s">
+        <v>222</v>
+      </c>
       <c r="D95" t="s">
         <v>22</v>
       </c>
@@ -7962,6 +8587,9 @@
       <c r="B96" t="s">
         <v>10</v>
       </c>
+      <c r="C96" t="s">
+        <v>221</v>
+      </c>
       <c r="D96" t="s">
         <v>22</v>
       </c>
@@ -7977,6 +8605,9 @@
       <c r="B97" t="s">
         <v>10</v>
       </c>
+      <c r="C97" t="s">
+        <v>117</v>
+      </c>
       <c r="D97" t="s">
         <v>22</v>
       </c>
@@ -7992,6 +8623,9 @@
       <c r="B98" t="s">
         <v>10</v>
       </c>
+      <c r="C98" t="s">
+        <v>223</v>
+      </c>
       <c r="D98" t="s">
         <v>22</v>
       </c>
@@ -8007,6 +8641,9 @@
       <c r="B99" t="s">
         <v>10</v>
       </c>
+      <c r="C99" t="s">
+        <v>224</v>
+      </c>
       <c r="D99" t="s">
         <v>22</v>
       </c>
@@ -8037,6 +8674,9 @@
       <c r="B101" t="s">
         <v>10</v>
       </c>
+      <c r="C101" t="s">
+        <v>184</v>
+      </c>
       <c r="D101" t="s">
         <v>22</v>
       </c>
@@ -8052,6 +8692,9 @@
       <c r="B102" t="s">
         <v>10</v>
       </c>
+      <c r="C102" t="s">
+        <v>225</v>
+      </c>
       <c r="D102" t="s">
         <v>22</v>
       </c>
@@ -8067,6 +8710,9 @@
       <c r="B103" t="s">
         <v>10</v>
       </c>
+      <c r="C103" t="s">
+        <v>226</v>
+      </c>
       <c r="D103" t="s">
         <v>22</v>
       </c>
@@ -8082,6 +8728,9 @@
       <c r="B104" t="s">
         <v>10</v>
       </c>
+      <c r="C104" t="s">
+        <v>227</v>
+      </c>
       <c r="D104" t="s">
         <v>22</v>
       </c>
@@ -8097,6 +8746,9 @@
       <c r="B105" t="s">
         <v>10</v>
       </c>
+      <c r="C105" t="s">
+        <v>228</v>
+      </c>
       <c r="D105" t="s">
         <v>22</v>
       </c>
@@ -8112,6 +8764,9 @@
       <c r="B106" t="s">
         <v>10</v>
       </c>
+      <c r="C106" t="s">
+        <v>229</v>
+      </c>
       <c r="D106" t="s">
         <v>22</v>
       </c>
@@ -8127,6 +8782,9 @@
       <c r="B107" t="s">
         <v>10</v>
       </c>
+      <c r="C107" t="s">
+        <v>230</v>
+      </c>
       <c r="D107" t="s">
         <v>22</v>
       </c>
@@ -8142,6 +8800,9 @@
       <c r="B108" t="s">
         <v>10</v>
       </c>
+      <c r="C108" t="s">
+        <v>231</v>
+      </c>
       <c r="D108" t="s">
         <v>22</v>
       </c>
@@ -8157,6 +8818,9 @@
       <c r="B109" t="s">
         <v>10</v>
       </c>
+      <c r="C109" t="s">
+        <v>232</v>
+      </c>
       <c r="D109" t="s">
         <v>22</v>
       </c>
@@ -8172,6 +8836,9 @@
       <c r="B110" t="s">
         <v>10</v>
       </c>
+      <c r="C110" t="s">
+        <v>233</v>
+      </c>
       <c r="D110" t="s">
         <v>22</v>
       </c>
@@ -8188,7 +8855,7 @@
         <v>10</v>
       </c>
       <c r="C111" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D111" t="s">
         <v>22</v>
@@ -8220,6 +8887,9 @@
       <c r="B113" t="s">
         <v>10</v>
       </c>
+      <c r="C113" t="s">
+        <v>234</v>
+      </c>
       <c r="D113" t="s">
         <v>22</v>
       </c>
@@ -8266,7 +8936,7 @@
         <v>10</v>
       </c>
       <c r="C116" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D116" t="s">
         <v>22</v>
@@ -8284,7 +8954,7 @@
         <v>10</v>
       </c>
       <c r="C117" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D117" t="s">
         <v>22</v>
@@ -8302,7 +8972,7 @@
         <v>10</v>
       </c>
       <c r="C118" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D118" t="s">
         <v>22</v>
@@ -8320,7 +8990,7 @@
         <v>10</v>
       </c>
       <c r="C119" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D119" t="s">
         <v>22</v>
@@ -8338,7 +9008,7 @@
         <v>10</v>
       </c>
       <c r="C120" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D120" t="s">
         <v>22</v>
@@ -8356,7 +9026,7 @@
         <v>10</v>
       </c>
       <c r="C121" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D121" t="s">
         <v>22</v>
@@ -8374,7 +9044,7 @@
         <v>10</v>
       </c>
       <c r="C122" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D122" t="s">
         <v>22</v>
@@ -8392,7 +9062,7 @@
         <v>10</v>
       </c>
       <c r="C123" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D123" t="s">
         <v>22</v>
@@ -8410,7 +9080,7 @@
         <v>10</v>
       </c>
       <c r="C124" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D124" t="s">
         <v>22</v>
@@ -8428,7 +9098,7 @@
         <v>10</v>
       </c>
       <c r="C125" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D125" t="s">
         <v>22</v>
@@ -8446,7 +9116,7 @@
         <v>10</v>
       </c>
       <c r="C126" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D126" t="s">
         <v>22</v>
@@ -8464,7 +9134,7 @@
         <v>10</v>
       </c>
       <c r="C127" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D127" t="s">
         <v>22</v>
@@ -8497,7 +9167,7 @@
         <v>10</v>
       </c>
       <c r="C129" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D129" t="s">
         <v>22</v>
@@ -8515,7 +9185,7 @@
         <v>10</v>
       </c>
       <c r="C130" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D130" t="s">
         <v>22</v>
@@ -8548,7 +9218,7 @@
         <v>10</v>
       </c>
       <c r="C132" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D132" t="s">
         <v>22</v>
@@ -8566,7 +9236,7 @@
         <v>10</v>
       </c>
       <c r="C133" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D133" t="s">
         <v>22</v>
@@ -8584,7 +9254,7 @@
         <v>10</v>
       </c>
       <c r="C134" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D134" t="s">
         <v>22</v>
@@ -8602,7 +9272,7 @@
         <v>10</v>
       </c>
       <c r="C135" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D135" t="s">
         <v>22</v>
@@ -8620,7 +9290,7 @@
         <v>10</v>
       </c>
       <c r="C136" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D136" t="s">
         <v>22</v>
@@ -8638,7 +9308,7 @@
         <v>10</v>
       </c>
       <c r="C137" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D137" t="s">
         <v>22</v>
@@ -8656,7 +9326,7 @@
         <v>10</v>
       </c>
       <c r="C138" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D138" t="s">
         <v>22</v>
@@ -8674,7 +9344,7 @@
         <v>10</v>
       </c>
       <c r="C139" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D139" t="s">
         <v>22</v>
@@ -8692,7 +9362,7 @@
         <v>10</v>
       </c>
       <c r="C140" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D140" t="s">
         <v>22</v>
@@ -8710,7 +9380,7 @@
         <v>10</v>
       </c>
       <c r="C141" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D141" t="s">
         <v>22</v>
@@ -8728,7 +9398,7 @@
         <v>10</v>
       </c>
       <c r="C142" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D142" t="s">
         <v>22</v>
@@ -8746,7 +9416,7 @@
         <v>10</v>
       </c>
       <c r="C143" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D143" t="s">
         <v>22</v>
@@ -8764,7 +9434,7 @@
         <v>10</v>
       </c>
       <c r="C144" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D144" t="s">
         <v>22</v>
@@ -8782,7 +9452,7 @@
         <v>10</v>
       </c>
       <c r="C145" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D145" t="s">
         <v>22</v>
@@ -8800,7 +9470,7 @@
         <v>10</v>
       </c>
       <c r="C146" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D146" t="s">
         <v>22</v>
@@ -8818,7 +9488,7 @@
         <v>10</v>
       </c>
       <c r="C147" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D147" t="s">
         <v>22</v>
@@ -8836,7 +9506,7 @@
         <v>10</v>
       </c>
       <c r="C148" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D148" t="s">
         <v>22</v>
@@ -8854,7 +9524,7 @@
         <v>10</v>
       </c>
       <c r="C149" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D149" t="s">
         <v>22</v>
@@ -8872,7 +9542,7 @@
         <v>10</v>
       </c>
       <c r="C150" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D150" t="s">
         <v>22</v>
@@ -8890,7 +9560,7 @@
         <v>10</v>
       </c>
       <c r="C151" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D151" t="s">
         <v>22</v>
@@ -8908,7 +9578,7 @@
         <v>10</v>
       </c>
       <c r="C152" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D152" t="s">
         <v>22</v>
@@ -8926,7 +9596,7 @@
         <v>10</v>
       </c>
       <c r="C153" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D153" t="s">
         <v>22</v>
@@ -8944,7 +9614,7 @@
         <v>10</v>
       </c>
       <c r="C154" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D154" t="s">
         <v>22</v>
@@ -8962,7 +9632,7 @@
         <v>10</v>
       </c>
       <c r="C155" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D155" t="s">
         <v>22</v>
@@ -8980,7 +9650,7 @@
         <v>10</v>
       </c>
       <c r="C156" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D156" t="s">
         <v>22</v>
@@ -8998,7 +9668,7 @@
         <v>10</v>
       </c>
       <c r="C157" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D157" t="s">
         <v>22</v>
@@ -9016,7 +9686,7 @@
         <v>10</v>
       </c>
       <c r="C158" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D158" t="s">
         <v>22</v>
@@ -9034,7 +9704,7 @@
         <v>10</v>
       </c>
       <c r="C159" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D159" t="s">
         <v>22</v>
@@ -9052,7 +9722,7 @@
         <v>10</v>
       </c>
       <c r="C160" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D160" t="s">
         <v>22</v>
@@ -9070,7 +9740,7 @@
         <v>10</v>
       </c>
       <c r="C161" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D161" t="s">
         <v>22</v>
@@ -9088,7 +9758,7 @@
         <v>10</v>
       </c>
       <c r="C162" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D162" t="s">
         <v>22</v>
@@ -9106,7 +9776,7 @@
         <v>10</v>
       </c>
       <c r="C163" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D163" t="s">
         <v>22</v>
@@ -9124,7 +9794,7 @@
         <v>10</v>
       </c>
       <c r="C164" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D164" t="s">
         <v>22</v>
@@ -9142,7 +9812,7 @@
         <v>10</v>
       </c>
       <c r="C165" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D165" t="s">
         <v>22</v>
@@ -9160,7 +9830,7 @@
         <v>10</v>
       </c>
       <c r="C166" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D166" t="s">
         <v>22</v>
@@ -9178,7 +9848,7 @@
         <v>10</v>
       </c>
       <c r="C167" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D167" t="s">
         <v>22</v>
@@ -9196,7 +9866,7 @@
         <v>10</v>
       </c>
       <c r="C168" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D168" t="s">
         <v>22</v>
@@ -9214,7 +9884,7 @@
         <v>10</v>
       </c>
       <c r="C169" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D169" t="s">
         <v>22</v>
@@ -9232,7 +9902,7 @@
         <v>10</v>
       </c>
       <c r="C170" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D170" t="s">
         <v>22</v>
@@ -9250,7 +9920,7 @@
         <v>10</v>
       </c>
       <c r="C171" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D171" t="s">
         <v>22</v>
@@ -9268,7 +9938,7 @@
         <v>10</v>
       </c>
       <c r="C172" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D172" t="s">
         <v>22</v>
@@ -9286,7 +9956,7 @@
         <v>10</v>
       </c>
       <c r="C173" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D173" t="s">
         <v>22</v>
@@ -9304,7 +9974,7 @@
         <v>10</v>
       </c>
       <c r="C174" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D174" t="s">
         <v>22</v>
@@ -9322,7 +9992,7 @@
         <v>10</v>
       </c>
       <c r="C175" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D175" t="s">
         <v>22</v>
@@ -9340,7 +10010,7 @@
         <v>10</v>
       </c>
       <c r="C176" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D176" t="s">
         <v>22</v>
@@ -9358,7 +10028,7 @@
         <v>10</v>
       </c>
       <c r="C177" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D177" t="s">
         <v>22</v>
@@ -9376,7 +10046,7 @@
         <v>10</v>
       </c>
       <c r="C178" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D178" t="s">
         <v>22</v>
@@ -9394,7 +10064,7 @@
         <v>10</v>
       </c>
       <c r="C179" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D179" t="s">
         <v>22</v>
@@ -9412,7 +10082,7 @@
         <v>10</v>
       </c>
       <c r="C180" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D180" t="s">
         <v>22</v>
@@ -9430,7 +10100,7 @@
         <v>10</v>
       </c>
       <c r="C181" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D181" t="s">
         <v>22</v>
@@ -9448,7 +10118,7 @@
         <v>10</v>
       </c>
       <c r="C182" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D182" t="s">
         <v>22</v>
@@ -9466,7 +10136,7 @@
         <v>10</v>
       </c>
       <c r="C183" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D183" t="s">
         <v>22</v>
@@ -9484,7 +10154,7 @@
         <v>10</v>
       </c>
       <c r="C184" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D184" t="s">
         <v>22</v>
@@ -9502,7 +10172,7 @@
         <v>10</v>
       </c>
       <c r="C185" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D185" t="s">
         <v>22</v>
@@ -9520,7 +10190,7 @@
         <v>10</v>
       </c>
       <c r="C186" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D186" t="s">
         <v>22</v>
@@ -9538,7 +10208,7 @@
         <v>10</v>
       </c>
       <c r="C187" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D187" t="s">
         <v>22</v>
@@ -9556,7 +10226,7 @@
         <v>10</v>
       </c>
       <c r="C188" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D188" t="s">
         <v>22</v>
@@ -9574,7 +10244,7 @@
         <v>10</v>
       </c>
       <c r="C189" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D189" t="s">
         <v>22</v>
@@ -9592,7 +10262,7 @@
         <v>10</v>
       </c>
       <c r="C190" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D190" t="s">
         <v>22</v>
@@ -9610,7 +10280,7 @@
         <v>10</v>
       </c>
       <c r="C191" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D191" t="s">
         <v>22</v>
@@ -9628,7 +10298,7 @@
         <v>10</v>
       </c>
       <c r="C192" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D192" t="s">
         <v>22</v>
@@ -9646,7 +10316,7 @@
         <v>10</v>
       </c>
       <c r="C193" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D193" t="s">
         <v>22</v>
@@ -9664,7 +10334,7 @@
         <v>10</v>
       </c>
       <c r="C194" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D194" t="s">
         <v>22</v>
@@ -9682,7 +10352,7 @@
         <v>10</v>
       </c>
       <c r="C195" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D195" t="s">
         <v>22</v>
@@ -9700,7 +10370,7 @@
         <v>10</v>
       </c>
       <c r="C196" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D196" t="s">
         <v>22</v>
@@ -9718,7 +10388,7 @@
         <v>10</v>
       </c>
       <c r="C197" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D197" t="s">
         <v>22</v>
@@ -9736,7 +10406,7 @@
         <v>10</v>
       </c>
       <c r="C198" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D198" t="s">
         <v>22</v>
@@ -9754,7 +10424,7 @@
         <v>10</v>
       </c>
       <c r="C199" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D199" t="s">
         <v>22</v>
@@ -9772,7 +10442,7 @@
         <v>10</v>
       </c>
       <c r="C200" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D200" t="s">
         <v>22</v>
@@ -9790,7 +10460,7 @@
         <v>10</v>
       </c>
       <c r="C201" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D201" t="s">
         <v>22</v>
@@ -9808,7 +10478,7 @@
         <v>10</v>
       </c>
       <c r="C202" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D202" t="s">
         <v>22</v>
@@ -9970,7 +10640,7 @@
         <v>10</v>
       </c>
       <c r="C211" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D211" t="s">
         <v>22</v>
@@ -9988,7 +10658,7 @@
         <v>10</v>
       </c>
       <c r="C212" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D212" t="s">
         <v>22</v>
@@ -10006,7 +10676,7 @@
         <v>10</v>
       </c>
       <c r="C213" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D213" t="s">
         <v>22</v>
@@ -10024,7 +10694,7 @@
         <v>10</v>
       </c>
       <c r="C214" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D214" t="s">
         <v>22</v>
@@ -10042,7 +10712,7 @@
         <v>10</v>
       </c>
       <c r="C215" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D215" t="s">
         <v>22</v>
@@ -10060,7 +10730,7 @@
         <v>10</v>
       </c>
       <c r="C216" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D216" t="s">
         <v>22</v>
@@ -10078,7 +10748,7 @@
         <v>10</v>
       </c>
       <c r="C217" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D217" t="s">
         <v>22</v>
@@ -10096,7 +10766,7 @@
         <v>10</v>
       </c>
       <c r="C218" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D218" t="s">
         <v>22</v>
@@ -10114,7 +10784,7 @@
         <v>10</v>
       </c>
       <c r="C219" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D219" t="s">
         <v>22</v>
@@ -10132,7 +10802,7 @@
         <v>10</v>
       </c>
       <c r="C220" t="s">
-        <v>37</v>
+        <v>213</v>
       </c>
       <c r="D220" t="s">
         <v>22</v>
@@ -10150,7 +10820,7 @@
         <v>10</v>
       </c>
       <c r="C221" t="s">
-        <v>38</v>
+        <v>212</v>
       </c>
       <c r="D221" t="s">
         <v>22</v>
@@ -10168,7 +10838,7 @@
         <v>10</v>
       </c>
       <c r="C222" t="s">
-        <v>39</v>
+        <v>214</v>
       </c>
       <c r="D222" t="s">
         <v>22</v>
@@ -10186,7 +10856,7 @@
         <v>10</v>
       </c>
       <c r="C223" t="s">
-        <v>40</v>
+        <v>211</v>
       </c>
       <c r="D223" t="s">
         <v>22</v>
@@ -10204,7 +10874,7 @@
         <v>10</v>
       </c>
       <c r="C224" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D224" t="s">
         <v>22</v>
@@ -10222,7 +10892,7 @@
         <v>10</v>
       </c>
       <c r="C225" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D225" t="s">
         <v>22</v>
@@ -10240,7 +10910,7 @@
         <v>10</v>
       </c>
       <c r="C226" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D226" t="s">
         <v>22</v>
@@ -10256,6 +10926,13 @@
       </c>
     </row>
   </sheetData>
+  <protectedRanges>
+    <protectedRange sqref="F1:F1048576" name="Alternatives"/>
+    <protectedRange sqref="L2:S9" name="Char Entry"/>
+    <protectedRange sqref="H1" name="Width"/>
+    <protectedRange sqref="C3:C226" name="Values"/>
+    <protectedRange sqref="E3:E226" name="Chars"/>
+  </protectedRanges>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>

</xml_diff>